<commit_message>
-[Exception To 100% To Print] functionality added. -Some required fields in RFQ Form done. (MOQs, Lead Times) -Fix: Delete RFQ from BOM Screen was not working for old RFQs (those with old EAU fashion).
</commit_message>
<xml_diff>
--- a/APQM Gantt.xlsx
+++ b/APQM Gantt.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="239">
   <si>
     <t>Plan</t>
   </si>
@@ -904,6 +904,12 @@
   <si>
     <t>Add LN column to BOM Screen</t>
   </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Download RFQ's Attachments do not work in Mozilla Firefox</t>
+  </si>
 </sst>
 </file>
 
@@ -912,7 +918,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -1070,12 +1076,6 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1427,38 +1427,38 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -4246,10 +4246,10 @@
   <dimension ref="A2:LK194"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="IZ175" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="J178" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="E184" sqref="E184"/>
+      <selection pane="bottomRight" activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -4266,11 +4266,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:323" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -4278,9 +4278,9 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="19" t="s">
         <v>13</v>
       </c>
@@ -4312,9 +4312,9 @@
       </c>
     </row>
     <row r="4" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="44"/>
       <c r="E4" s="32"/>
       <c r="F4" s="18"/>
@@ -13245,11 +13245,11 @@
       <c r="LK69" s="28"/>
     </row>
     <row r="70" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="67" t="s">
+      <c r="A70" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="67"/>
-      <c r="C70" s="67"/>
+      <c r="B70" s="66"/>
+      <c r="C70" s="66"/>
       <c r="D70" s="29"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -14397,10 +14397,10 @@
       <c r="C80" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="D80" s="60" t="s">
+      <c r="D80" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="E80" s="59"/>
+      <c r="E80" s="58"/>
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
       <c r="H80" s="5">
@@ -15018,11 +15018,11 @@
       <c r="LK85" s="28"/>
     </row>
     <row r="86" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="67" t="s">
+      <c r="A86" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="B86" s="67"/>
-      <c r="C86" s="67"/>
+      <c r="B86" s="66"/>
+      <c r="C86" s="66"/>
       <c r="D86" s="29"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -19299,11 +19299,11 @@
       <c r="LK124" s="28"/>
     </row>
     <row r="125" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="67" t="s">
+      <c r="A125" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="B125" s="67"/>
-      <c r="C125" s="67"/>
+      <c r="B125" s="66"/>
+      <c r="C125" s="66"/>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
@@ -21848,7 +21848,7 @@
       <c r="B148" s="26">
         <v>2</v>
       </c>
-      <c r="C148" s="61" t="s">
+      <c r="C148" s="53" t="s">
         <v>148</v>
       </c>
       <c r="D148" s="29">
@@ -23616,10 +23616,10 @@
       <c r="A164" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="B164" s="67" t="s">
+      <c r="B164" s="66" t="s">
         <v>225</v>
       </c>
-      <c r="C164" s="67"/>
+      <c r="C164" s="66"/>
       <c r="D164" s="29"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
@@ -23831,7 +23831,7 @@
       <c r="B166" s="26">
         <v>5</v>
       </c>
-      <c r="C166" s="53" t="s">
+      <c r="C166" s="55" t="s">
         <v>201</v>
       </c>
       <c r="D166" s="29"/>
@@ -23944,7 +23944,7 @@
       <c r="B167" s="26">
         <v>5</v>
       </c>
-      <c r="C167" s="53" t="s">
+      <c r="C167" s="55" t="s">
         <v>223</v>
       </c>
       <c r="D167" s="29"/>
@@ -24054,7 +24054,7 @@
       <c r="B168" s="26">
         <v>5</v>
       </c>
-      <c r="C168" s="58" t="s">
+      <c r="C168" s="68" t="s">
         <v>208</v>
       </c>
       <c r="D168" s="29"/>
@@ -24167,7 +24167,7 @@
       <c r="B169" s="26">
         <v>5</v>
       </c>
-      <c r="C169" s="58" t="s">
+      <c r="C169" s="68" t="s">
         <v>209</v>
       </c>
       <c r="D169" s="29"/>
@@ -24280,7 +24280,7 @@
       <c r="B170" s="26">
         <v>5</v>
       </c>
-      <c r="C170" s="58" t="s">
+      <c r="C170" s="68" t="s">
         <v>210</v>
       </c>
       <c r="D170" s="29"/>
@@ -24393,7 +24393,7 @@
       <c r="B171" s="26">
         <v>5</v>
       </c>
-      <c r="C171" s="58" t="s">
+      <c r="C171" s="68" t="s">
         <v>216</v>
       </c>
       <c r="D171" s="29"/>
@@ -24506,7 +24506,7 @@
       <c r="B172" s="26">
         <v>5</v>
       </c>
-      <c r="C172" s="58" t="s">
+      <c r="C172" s="68" t="s">
         <v>215</v>
       </c>
       <c r="D172" s="29"/>
@@ -24617,7 +24617,7 @@
       <c r="B173" s="26">
         <v>5</v>
       </c>
-      <c r="C173" s="58" t="s">
+      <c r="C173" s="68" t="s">
         <v>217</v>
       </c>
       <c r="D173" s="29"/>
@@ -24730,7 +24730,7 @@
       <c r="B174" s="26">
         <v>5</v>
       </c>
-      <c r="C174" s="58" t="s">
+      <c r="C174" s="68" t="s">
         <v>219</v>
       </c>
       <c r="D174" s="29"/>
@@ -24842,7 +24842,7 @@
       <c r="B175" s="26">
         <v>5</v>
       </c>
-      <c r="C175" s="58" t="s">
+      <c r="C175" s="68" t="s">
         <v>218</v>
       </c>
       <c r="D175" s="29"/>
@@ -24954,7 +24954,7 @@
       <c r="B176" s="26">
         <v>5</v>
       </c>
-      <c r="C176" s="58" t="s">
+      <c r="C176" s="68" t="s">
         <v>220</v>
       </c>
       <c r="D176" s="29"/>
@@ -25067,7 +25067,7 @@
       <c r="B177" s="26">
         <v>5</v>
       </c>
-      <c r="C177" s="53" t="s">
+      <c r="C177" s="55" t="s">
         <v>213</v>
       </c>
       <c r="D177" s="29"/>
@@ -25146,7 +25146,7 @@
       <c r="HQ177" s="28"/>
       <c r="HW177" s="28"/>
       <c r="HX177" s="28"/>
-      <c r="HY177" s="59"/>
+      <c r="HY177" s="58"/>
       <c r="ID177" s="28"/>
       <c r="IE177" s="28"/>
       <c r="IK177" s="28"/>
@@ -25180,7 +25180,7 @@
       <c r="B178" s="26">
         <v>5</v>
       </c>
-      <c r="C178" s="53" t="s">
+      <c r="C178" s="55" t="s">
         <v>211</v>
       </c>
       <c r="D178" s="29"/>
@@ -25293,7 +25293,7 @@
       <c r="B179" s="26">
         <v>5</v>
       </c>
-      <c r="C179" s="53" t="s">
+      <c r="C179" s="55" t="s">
         <v>214</v>
       </c>
       <c r="D179" s="29"/>
@@ -25406,7 +25406,7 @@
       <c r="B180" s="26">
         <v>5</v>
       </c>
-      <c r="C180" s="53" t="s">
+      <c r="C180" s="55" t="s">
         <v>221</v>
       </c>
       <c r="D180" s="29"/>
@@ -25519,7 +25519,7 @@
       <c r="B181" s="26">
         <v>5</v>
       </c>
-      <c r="C181" s="53" t="s">
+      <c r="C181" s="55" t="s">
         <v>222</v>
       </c>
       <c r="D181" s="29"/>
@@ -25644,7 +25644,7 @@
       <c r="F182" s="13"/>
       <c r="G182" s="13"/>
       <c r="H182" s="5">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="N182" s="28"/>
       <c r="O182" s="28"/>
@@ -27241,7 +27241,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27321,7 +27321,7 @@
       <c r="D6" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="62"/>
+      <c r="E6" s="60"/>
       <c r="AO6" s="35" t="s">
         <v>59</v>
       </c>
@@ -27470,7 +27470,19 @@
       <c r="A14" s="36">
         <v>10</v>
       </c>
-      <c r="B14" s="66"/>
+      <c r="B14" s="64">
+        <v>41810</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="65"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="36">
@@ -27486,11 +27498,11 @@
       <c r="A17" s="36">
         <v>13</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="64"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="62"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="36">

</xml_diff>

<commit_message>
-Change BOM Component status back to 'In Progress' when its Awarded or Selected RFQ has been deleted. -Fix: Popup in RFQ Summary was not refreshing now painting in yellow. -In Progress: Prevent from deletiting records, just set them to inactive, so that we wont delete any data in our database and we'll be able to restore data.
</commit_message>
<xml_diff>
--- a/APQM Gantt.xlsx
+++ b/APQM Gantt.xlsx
@@ -872,9 +872,6 @@
     <t>New tasks added since May</t>
   </si>
   <si>
-    <t>Ordered by Actual Start. LMD: 6/9/2014</t>
-  </si>
-  <si>
     <t>At the end</t>
   </si>
   <si>
@@ -903,6 +900,9 @@
   </si>
   <si>
     <t>Add LN column to BOM Screen</t>
+  </si>
+  <si>
+    <t>Ordered by Actual Start. LMD: 6/24/2014</t>
   </si>
 </sst>
 </file>
@@ -1427,9 +1427,6 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1459,6 +1456,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -4246,10 +4246,10 @@
   <dimension ref="A2:LK194"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="IZ171" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="IZ129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F182" sqref="F182"/>
+      <selection pane="bottomRight" activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -4266,11 +4266,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:323" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -4278,15 +4278,15 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3">
-        <v>155</v>
+        <v>260</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -4312,9 +4312,9 @@
       </c>
     </row>
     <row r="4" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="44"/>
       <c r="E4" s="32"/>
       <c r="F4" s="18"/>
@@ -4323,7 +4323,7 @@
     </row>
     <row r="5" spans="1:323" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="15"/>
@@ -13245,11 +13245,11 @@
       <c r="LK69" s="28"/>
     </row>
     <row r="70" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="67" t="s">
+      <c r="A70" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="67"/>
-      <c r="C70" s="67"/>
+      <c r="B70" s="66"/>
+      <c r="C70" s="66"/>
       <c r="D70" s="29"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -14397,10 +14397,10 @@
       <c r="C80" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="D80" s="60" t="s">
-        <v>227</v>
-      </c>
-      <c r="E80" s="59"/>
+      <c r="D80" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="E80" s="58"/>
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
       <c r="H80" s="5">
@@ -15018,11 +15018,11 @@
       <c r="LK85" s="28"/>
     </row>
     <row r="86" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="67" t="s">
+      <c r="A86" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="B86" s="67"/>
-      <c r="C86" s="67"/>
+      <c r="B86" s="66"/>
+      <c r="C86" s="66"/>
       <c r="D86" s="29"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -19299,11 +19299,11 @@
       <c r="LK124" s="28"/>
     </row>
     <row r="125" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="67" t="s">
+      <c r="A125" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="B125" s="67"/>
-      <c r="C125" s="67"/>
+      <c r="B125" s="66"/>
+      <c r="C125" s="66"/>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
@@ -19961,7 +19961,7 @@
       <c r="B131" s="26">
         <v>5</v>
       </c>
-      <c r="C131" s="53" t="s">
+      <c r="C131" s="55" t="s">
         <v>152</v>
       </c>
       <c r="D131" s="29">
@@ -19970,10 +19970,14 @@
       <c r="E131" s="13">
         <v>1</v>
       </c>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
+      <c r="F131" s="13">
+        <v>260</v>
+      </c>
+      <c r="G131" s="13">
+        <v>1</v>
+      </c>
       <c r="H131" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N131" s="28"/>
       <c r="O131" s="28"/>
@@ -20081,8 +20085,12 @@
       <c r="E132" s="13">
         <v>4</v>
       </c>
-      <c r="F132" s="13"/>
-      <c r="G132" s="13"/>
+      <c r="F132" s="13">
+        <v>260</v>
+      </c>
+      <c r="G132" s="13">
+        <v>1</v>
+      </c>
       <c r="H132" s="5">
         <v>0</v>
       </c>
@@ -21848,7 +21856,7 @@
       <c r="B148" s="26">
         <v>2</v>
       </c>
-      <c r="C148" s="61" t="s">
+      <c r="C148" s="60" t="s">
         <v>148</v>
       </c>
       <c r="D148" s="29">
@@ -23616,10 +23624,10 @@
       <c r="A164" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="B164" s="67" t="s">
+      <c r="B164" s="66" t="s">
         <v>225</v>
       </c>
-      <c r="C164" s="67"/>
+      <c r="C164" s="66"/>
       <c r="D164" s="29"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
@@ -23831,7 +23839,7 @@
       <c r="B166" s="26">
         <v>5</v>
       </c>
-      <c r="C166" s="53" t="s">
+      <c r="C166" s="55" t="s">
         <v>201</v>
       </c>
       <c r="D166" s="29"/>
@@ -23944,7 +23952,7 @@
       <c r="B167" s="26">
         <v>5</v>
       </c>
-      <c r="C167" s="53" t="s">
+      <c r="C167" s="55" t="s">
         <v>223</v>
       </c>
       <c r="D167" s="29"/>
@@ -24054,7 +24062,7 @@
       <c r="B168" s="26">
         <v>5</v>
       </c>
-      <c r="C168" s="58" t="s">
+      <c r="C168" s="68" t="s">
         <v>208</v>
       </c>
       <c r="D168" s="29"/>
@@ -24167,7 +24175,7 @@
       <c r="B169" s="26">
         <v>5</v>
       </c>
-      <c r="C169" s="58" t="s">
+      <c r="C169" s="68" t="s">
         <v>209</v>
       </c>
       <c r="D169" s="29"/>
@@ -24280,7 +24288,7 @@
       <c r="B170" s="26">
         <v>5</v>
       </c>
-      <c r="C170" s="58" t="s">
+      <c r="C170" s="68" t="s">
         <v>210</v>
       </c>
       <c r="D170" s="29"/>
@@ -24393,7 +24401,7 @@
       <c r="B171" s="26">
         <v>5</v>
       </c>
-      <c r="C171" s="58" t="s">
+      <c r="C171" s="68" t="s">
         <v>216</v>
       </c>
       <c r="D171" s="29"/>
@@ -24506,7 +24514,7 @@
       <c r="B172" s="26">
         <v>5</v>
       </c>
-      <c r="C172" s="58" t="s">
+      <c r="C172" s="68" t="s">
         <v>215</v>
       </c>
       <c r="D172" s="29"/>
@@ -24617,7 +24625,7 @@
       <c r="B173" s="26">
         <v>5</v>
       </c>
-      <c r="C173" s="58" t="s">
+      <c r="C173" s="68" t="s">
         <v>217</v>
       </c>
       <c r="D173" s="29"/>
@@ -24730,7 +24738,7 @@
       <c r="B174" s="26">
         <v>5</v>
       </c>
-      <c r="C174" s="58" t="s">
+      <c r="C174" s="68" t="s">
         <v>219</v>
       </c>
       <c r="D174" s="29"/>
@@ -24842,7 +24850,7 @@
       <c r="B175" s="26">
         <v>5</v>
       </c>
-      <c r="C175" s="58" t="s">
+      <c r="C175" s="68" t="s">
         <v>218</v>
       </c>
       <c r="D175" s="29"/>
@@ -24954,7 +24962,7 @@
       <c r="B176" s="26">
         <v>5</v>
       </c>
-      <c r="C176" s="58" t="s">
+      <c r="C176" s="68" t="s">
         <v>220</v>
       </c>
       <c r="D176" s="29"/>
@@ -25067,7 +25075,7 @@
       <c r="B177" s="26">
         <v>5</v>
       </c>
-      <c r="C177" s="53" t="s">
+      <c r="C177" s="55" t="s">
         <v>213</v>
       </c>
       <c r="D177" s="29"/>
@@ -25146,7 +25154,7 @@
       <c r="HQ177" s="28"/>
       <c r="HW177" s="28"/>
       <c r="HX177" s="28"/>
-      <c r="HY177" s="59"/>
+      <c r="HY177" s="58"/>
       <c r="ID177" s="28"/>
       <c r="IE177" s="28"/>
       <c r="IK177" s="28"/>
@@ -25180,7 +25188,7 @@
       <c r="B178" s="26">
         <v>5</v>
       </c>
-      <c r="C178" s="53" t="s">
+      <c r="C178" s="55" t="s">
         <v>211</v>
       </c>
       <c r="D178" s="29"/>
@@ -25293,7 +25301,7 @@
       <c r="B179" s="26">
         <v>5</v>
       </c>
-      <c r="C179" s="53" t="s">
+      <c r="C179" s="55" t="s">
         <v>214</v>
       </c>
       <c r="D179" s="29"/>
@@ -25406,7 +25414,7 @@
       <c r="B180" s="26">
         <v>5</v>
       </c>
-      <c r="C180" s="53" t="s">
+      <c r="C180" s="55" t="s">
         <v>221</v>
       </c>
       <c r="D180" s="29"/>
@@ -25519,7 +25527,7 @@
       <c r="B181" s="26">
         <v>5</v>
       </c>
-      <c r="C181" s="53" t="s">
+      <c r="C181" s="55" t="s">
         <v>222</v>
       </c>
       <c r="D181" s="29"/>
@@ -25632,7 +25640,7 @@
       <c r="B182" s="26">
         <v>5</v>
       </c>
-      <c r="C182" s="53" t="s">
+      <c r="C182" s="55" t="s">
         <v>224</v>
       </c>
       <c r="D182" s="29">
@@ -25845,13 +25853,13 @@
     </row>
     <row r="184" spans="1:323" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B184" s="26">
         <v>3</v>
       </c>
       <c r="C184" s="53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="13">
@@ -25960,7 +25968,7 @@
         <v>3</v>
       </c>
       <c r="C185" s="53" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="13">
@@ -26069,7 +26077,7 @@
         <v>3</v>
       </c>
       <c r="C186" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="13">
@@ -26178,7 +26186,7 @@
         <v>3</v>
       </c>
       <c r="C187" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="13">
@@ -26287,7 +26295,7 @@
         <v>3</v>
       </c>
       <c r="C188" s="53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="13">
@@ -26396,7 +26404,7 @@
         <v>3</v>
       </c>
       <c r="C189" s="53" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="13">
@@ -27325,7 +27333,7 @@
       <c r="D6" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="62"/>
+      <c r="E6" s="61"/>
       <c r="AO6" s="35" t="s">
         <v>59</v>
       </c>
@@ -27461,20 +27469,20 @@
         <v>161</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="36">
         <v>10</v>
       </c>
-      <c r="B14" s="66"/>
+      <c r="B14" s="65"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="36">
@@ -27490,11 +27498,11 @@
       <c r="A17" s="36">
         <v>13</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="64"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="63"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="36">

</xml_diff>

<commit_message>
-Inactive records instead of delete them.
</commit_message>
<xml_diff>
--- a/APQM Gantt.xlsx
+++ b/APQM Gantt.xlsx
@@ -1451,14 +1451,14 @@
     <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -3943,7 +3943,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="155" min="1" page="10" val="155"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="500" min="1" page="10" val="261"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4246,10 +4246,10 @@
   <dimension ref="A2:LK194"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="IZ129" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="JE131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="I133" sqref="I133"/>
+      <selection pane="bottomRight" activeCell="JJ132" sqref="JJ132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -4266,11 +4266,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:323" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -4278,15 +4278,15 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -4312,9 +4312,9 @@
       </c>
     </row>
     <row r="4" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="44"/>
       <c r="E4" s="32"/>
       <c r="F4" s="18"/>
@@ -13245,11 +13245,11 @@
       <c r="LK69" s="28"/>
     </row>
     <row r="70" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="66" t="s">
+      <c r="A70" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="66"/>
-      <c r="C70" s="66"/>
+      <c r="B70" s="67"/>
+      <c r="C70" s="67"/>
       <c r="D70" s="29"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -15018,11 +15018,11 @@
       <c r="LK85" s="28"/>
     </row>
     <row r="86" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="66" t="s">
+      <c r="A86" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="B86" s="66"/>
-      <c r="C86" s="66"/>
+      <c r="B86" s="67"/>
+      <c r="C86" s="67"/>
       <c r="D86" s="29"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -19299,11 +19299,11 @@
       <c r="LK124" s="28"/>
     </row>
     <row r="125" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="66" t="s">
+      <c r="A125" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="B125" s="66"/>
-      <c r="C125" s="66"/>
+      <c r="B125" s="67"/>
+      <c r="C125" s="67"/>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
@@ -20076,7 +20076,7 @@
       <c r="B132" s="26">
         <v>5</v>
       </c>
-      <c r="C132" s="53" t="s">
+      <c r="C132" s="55" t="s">
         <v>163</v>
       </c>
       <c r="D132" s="29">
@@ -20089,10 +20089,10 @@
         <v>260</v>
       </c>
       <c r="G132" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H132" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N132" s="28"/>
       <c r="O132" s="28"/>
@@ -23624,10 +23624,10 @@
       <c r="A164" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="B164" s="66" t="s">
+      <c r="B164" s="67" t="s">
         <v>225</v>
       </c>
-      <c r="C164" s="66"/>
+      <c r="C164" s="67"/>
       <c r="D164" s="29"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
@@ -24062,7 +24062,7 @@
       <c r="B168" s="26">
         <v>5</v>
       </c>
-      <c r="C168" s="68" t="s">
+      <c r="C168" s="66" t="s">
         <v>208</v>
       </c>
       <c r="D168" s="29"/>
@@ -24175,7 +24175,7 @@
       <c r="B169" s="26">
         <v>5</v>
       </c>
-      <c r="C169" s="68" t="s">
+      <c r="C169" s="66" t="s">
         <v>209</v>
       </c>
       <c r="D169" s="29"/>
@@ -24288,7 +24288,7 @@
       <c r="B170" s="26">
         <v>5</v>
       </c>
-      <c r="C170" s="68" t="s">
+      <c r="C170" s="66" t="s">
         <v>210</v>
       </c>
       <c r="D170" s="29"/>
@@ -24401,7 +24401,7 @@
       <c r="B171" s="26">
         <v>5</v>
       </c>
-      <c r="C171" s="68" t="s">
+      <c r="C171" s="66" t="s">
         <v>216</v>
       </c>
       <c r="D171" s="29"/>
@@ -24514,7 +24514,7 @@
       <c r="B172" s="26">
         <v>5</v>
       </c>
-      <c r="C172" s="68" t="s">
+      <c r="C172" s="66" t="s">
         <v>215</v>
       </c>
       <c r="D172" s="29"/>
@@ -24625,7 +24625,7 @@
       <c r="B173" s="26">
         <v>5</v>
       </c>
-      <c r="C173" s="68" t="s">
+      <c r="C173" s="66" t="s">
         <v>217</v>
       </c>
       <c r="D173" s="29"/>
@@ -24738,7 +24738,7 @@
       <c r="B174" s="26">
         <v>5</v>
       </c>
-      <c r="C174" s="68" t="s">
+      <c r="C174" s="66" t="s">
         <v>219</v>
       </c>
       <c r="D174" s="29"/>
@@ -24850,7 +24850,7 @@
       <c r="B175" s="26">
         <v>5</v>
       </c>
-      <c r="C175" s="68" t="s">
+      <c r="C175" s="66" t="s">
         <v>218</v>
       </c>
       <c r="D175" s="29"/>
@@ -24962,7 +24962,7 @@
       <c r="B176" s="26">
         <v>5</v>
       </c>
-      <c r="C176" s="68" t="s">
+      <c r="C176" s="66" t="s">
         <v>220</v>
       </c>
       <c r="D176" s="29"/>

</xml_diff>

<commit_message>
Change bom status to in progress only when delete rfq seletected/awarded
</commit_message>
<xml_diff>
--- a/APQM Gantt.xlsx
+++ b/APQM Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
+    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="APQM Gantt" sheetId="2" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="238">
   <si>
     <t>Plan</t>
   </si>
@@ -903,6 +903,9 @@
   </si>
   <si>
     <t>Ordered by Actual Start. LMD: 6/24/2014</t>
+  </si>
+  <si>
+    <t>HTML Report summing all eaus</t>
   </si>
 </sst>
 </file>
@@ -4245,11 +4248,11 @@
   </sheetPr>
   <dimension ref="A2:LK194"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
       <pane xSplit="9" ySplit="7" topLeftCell="JE131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="JJ132" sqref="JJ132"/>
+      <selection pane="bottomRight" activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -27251,9 +27254,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AO238"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27482,7 +27485,15 @@
       <c r="A14" s="36">
         <v>10</v>
       </c>
-      <c r="B14" s="65"/>
+      <c r="B14" s="65">
+        <v>41815</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="36">

</xml_diff>

<commit_message>
-Remove old Lead Time fields. -Include UM field to importation proess in SalesDB2APQM.exe. -Reports: All RFQs and RFQs selected/awarded using EAVStatus.
</commit_message>
<xml_diff>
--- a/APQM Gantt.xlsx
+++ b/APQM Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350" activeTab="1"/>
+    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
   </bookViews>
   <sheets>
     <sheet name="APQM Gantt" sheetId="2" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="240">
   <si>
     <t>Plan</t>
   </si>
@@ -650,9 +650,6 @@
     <t>See issue with NDA</t>
   </si>
   <si>
-    <t>Change BOM Component status when its RFQ award/selected has been deleted</t>
-  </si>
-  <si>
     <t>Page inside emails</t>
   </si>
   <si>
@@ -902,10 +899,19 @@
     <t>Add LN column to BOM Screen</t>
   </si>
   <si>
-    <t>Ordered by Actual Start. LMD: 6/24/2014</t>
+    <t>HTML Report summing all eaus</t>
   </si>
   <si>
-    <t>HTML Report summing all eaus</t>
+    <t>Not programmed</t>
+  </si>
+  <si>
+    <t>Ordered by Actual Start. LMD: 7/1/2014</t>
+  </si>
+  <si>
+    <t>to be able to quote some component that was before estimated, but not remove the estimated information</t>
+  </si>
+  <si>
+    <t>Add UM to Sales DB so then, it can be imported to APQM</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1263,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1456,6 +1462,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3946,7 +3955,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="500" min="1" page="10" val="261"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="500" min="1" page="10" val="268"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4246,13 +4255,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:LK194"/>
+  <dimension ref="A2:LK208"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="JE131" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane xSplit="9" ySplit="7" topLeftCell="JL190" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C133" sqref="C133"/>
+      <selection pane="bottomRight" activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -4269,11 +4278,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:323" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -4281,15 +4290,15 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
       <c r="D3" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -4315,9 +4324,9 @@
       </c>
     </row>
     <row r="4" spans="1:323" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="44"/>
       <c r="E4" s="32"/>
       <c r="F4" s="18"/>
@@ -4326,7 +4335,7 @@
     </row>
     <row r="5" spans="1:323" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="15"/>
@@ -13248,11 +13257,11 @@
       <c r="LK69" s="28"/>
     </row>
     <row r="70" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="67" t="s">
+      <c r="A70" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="67"/>
-      <c r="C70" s="67"/>
+      <c r="B70" s="68"/>
+      <c r="C70" s="68"/>
       <c r="D70" s="29"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -14401,7 +14410,7 @@
         <v>128</v>
       </c>
       <c r="D80" s="59" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E80" s="58"/>
       <c r="F80" s="13"/>
@@ -15021,11 +15030,11 @@
       <c r="LK85" s="28"/>
     </row>
     <row r="86" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="67" t="s">
+      <c r="A86" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="B86" s="67"/>
-      <c r="C86" s="67"/>
+      <c r="B86" s="68"/>
+      <c r="C86" s="68"/>
       <c r="D86" s="29"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -15893,7 +15902,7 @@
       <c r="LJ93" s="28"/>
       <c r="LK93" s="28"/>
     </row>
-    <row r="94" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:323" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="25"/>
       <c r="B94" s="26">
         <v>5</v>
@@ -18225,7 +18234,7 @@
       <c r="A115" s="25"/>
       <c r="B115" s="26"/>
       <c r="C115" s="52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="13">
@@ -18336,7 +18345,7 @@
       <c r="A116" s="25"/>
       <c r="B116" s="26"/>
       <c r="C116" s="52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="13"/>
@@ -18445,7 +18454,7 @@
       <c r="A117" s="25"/>
       <c r="B117" s="26"/>
       <c r="C117" s="52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="13"/>
@@ -18554,7 +18563,7 @@
       <c r="A118" s="25"/>
       <c r="B118" s="26"/>
       <c r="C118" s="52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="13"/>
@@ -18663,7 +18672,7 @@
       <c r="A119" s="25"/>
       <c r="B119" s="26"/>
       <c r="C119" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="13"/>
@@ -18772,7 +18781,7 @@
       <c r="A120" s="25"/>
       <c r="B120" s="26"/>
       <c r="C120" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D120" s="29">
         <v>116</v>
@@ -18885,7 +18894,7 @@
       <c r="A121" s="25"/>
       <c r="B121" s="26"/>
       <c r="C121" s="52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="13"/>
@@ -18994,7 +19003,7 @@
       <c r="A122" s="25"/>
       <c r="B122" s="26"/>
       <c r="C122" s="52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="13"/>
@@ -19302,11 +19311,11 @@
       <c r="LK124" s="28"/>
     </row>
     <row r="125" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="67" t="s">
+      <c r="A125" s="68" t="s">
         <v>146</v>
       </c>
-      <c r="B125" s="67"/>
-      <c r="C125" s="67"/>
+      <c r="B125" s="68"/>
+      <c r="C125" s="68"/>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
@@ -19410,7 +19419,7 @@
         <v>5</v>
       </c>
       <c r="C126" s="55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="13"/>
@@ -19521,7 +19530,7 @@
         <v>5</v>
       </c>
       <c r="C127" s="55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="13"/>
@@ -19632,7 +19641,7 @@
         <v>5</v>
       </c>
       <c r="C128" s="55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="13"/>
@@ -19743,7 +19752,7 @@
         <v>4</v>
       </c>
       <c r="C129" s="55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="13"/>
@@ -19853,8 +19862,8 @@
       <c r="B130" s="26">
         <v>4</v>
       </c>
-      <c r="C130" s="53" t="s">
-        <v>166</v>
+      <c r="C130" s="55" t="s">
+        <v>165</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="13"/>
@@ -19965,7 +19974,7 @@
         <v>5</v>
       </c>
       <c r="C131" s="55" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="D131" s="29">
         <v>256</v>
@@ -20080,7 +20089,7 @@
         <v>5</v>
       </c>
       <c r="C132" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D132" s="29">
         <v>256</v>
@@ -20195,7 +20204,7 @@
         <v>5</v>
       </c>
       <c r="C133" s="53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D133" s="29">
         <v>259</v>
@@ -20306,7 +20315,7 @@
         <v>4</v>
       </c>
       <c r="C134" s="53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D134" s="29">
         <v>260</v>
@@ -20417,7 +20426,7 @@
         <v>4</v>
       </c>
       <c r="C135" s="53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D135" s="29">
         <v>260</v>
@@ -20528,7 +20537,7 @@
         <v>4</v>
       </c>
       <c r="C136" s="53" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D136" s="29">
         <v>260</v>
@@ -20639,7 +20648,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D137" s="29">
         <v>261</v>
@@ -20861,7 +20870,7 @@
         <v>3</v>
       </c>
       <c r="C139" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D139" s="29">
         <v>262</v>
@@ -20972,7 +20981,7 @@
         <v>3</v>
       </c>
       <c r="C140" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D140" s="29">
         <v>262</v>
@@ -21083,7 +21092,7 @@
         <v>3</v>
       </c>
       <c r="C141" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D141" s="29">
         <v>263</v>
@@ -21194,7 +21203,7 @@
         <v>3</v>
       </c>
       <c r="C142" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D142" s="29">
         <v>263</v>
@@ -21305,7 +21314,7 @@
         <v>3</v>
       </c>
       <c r="C143" s="53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D143" s="29">
         <v>266</v>
@@ -21416,7 +21425,7 @@
         <v>3</v>
       </c>
       <c r="C144" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D144" s="29">
         <v>266</v>
@@ -21527,7 +21536,7 @@
         <v>3</v>
       </c>
       <c r="C145" s="53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D145" s="29">
         <v>268</v>
@@ -21638,7 +21647,7 @@
         <v>3</v>
       </c>
       <c r="C146" s="53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D146" s="29">
         <v>268</v>
@@ -21749,7 +21758,7 @@
         <v>3</v>
       </c>
       <c r="C147" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D147" s="29">
         <v>269</v>
@@ -21971,7 +21980,7 @@
         <v>2</v>
       </c>
       <c r="C149" s="53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D149" s="29">
         <v>281</v>
@@ -22082,7 +22091,7 @@
         <v>2</v>
       </c>
       <c r="C150" s="53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D150" s="29">
         <v>287</v>
@@ -22304,7 +22313,7 @@
         <v>2</v>
       </c>
       <c r="C152" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D152" s="29">
         <v>289</v>
@@ -22415,7 +22424,7 @@
         <v>2</v>
       </c>
       <c r="C153" s="53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D153" s="29">
         <v>290</v>
@@ -22526,7 +22535,7 @@
         <v>2</v>
       </c>
       <c r="C154" s="53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D154" s="29">
         <v>290</v>
@@ -22637,7 +22646,7 @@
         <v>2</v>
       </c>
       <c r="C155" s="53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D155" s="29">
         <v>294</v>
@@ -22970,7 +22979,7 @@
         <v>1</v>
       </c>
       <c r="C158" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D158" s="29">
         <v>296</v>
@@ -23625,12 +23634,12 @@
     </row>
     <row r="164" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="57" t="s">
-        <v>202</v>
-      </c>
-      <c r="B164" s="67" t="s">
-        <v>225</v>
-      </c>
-      <c r="C164" s="67"/>
+        <v>201</v>
+      </c>
+      <c r="B164" s="68" t="s">
+        <v>224</v>
+      </c>
+      <c r="C164" s="68"/>
       <c r="D164" s="29"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
@@ -23730,13 +23739,13 @@
     </row>
     <row r="165" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B165" s="26">
         <v>3</v>
       </c>
       <c r="C165" s="53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="13"/>
@@ -23837,13 +23846,13 @@
     </row>
     <row r="166" spans="1:323" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B166" s="26">
         <v>5</v>
       </c>
       <c r="C166" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D166" s="29"/>
       <c r="E166" s="13"/>
@@ -23950,13 +23959,13 @@
     </row>
     <row r="167" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B167" s="26">
         <v>5</v>
       </c>
       <c r="C167" s="55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="13"/>
@@ -24060,13 +24069,13 @@
     </row>
     <row r="168" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B168" s="26">
         <v>5</v>
       </c>
       <c r="C168" s="66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D168" s="29"/>
       <c r="E168" s="13"/>
@@ -24173,13 +24182,13 @@
     </row>
     <row r="169" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B169" s="26">
         <v>5</v>
       </c>
       <c r="C169" s="66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="13"/>
@@ -24286,13 +24295,13 @@
     </row>
     <row r="170" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B170" s="26">
         <v>5</v>
       </c>
       <c r="C170" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D170" s="29"/>
       <c r="E170" s="13"/>
@@ -24399,13 +24408,13 @@
     </row>
     <row r="171" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B171" s="26">
         <v>5</v>
       </c>
       <c r="C171" s="66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D171" s="29"/>
       <c r="E171" s="13"/>
@@ -24512,13 +24521,13 @@
     </row>
     <row r="172" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B172" s="26">
         <v>5</v>
       </c>
       <c r="C172" s="66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="13"/>
@@ -24623,13 +24632,13 @@
     </row>
     <row r="173" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B173" s="26">
         <v>5</v>
       </c>
       <c r="C173" s="66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="13"/>
@@ -24736,13 +24745,13 @@
     </row>
     <row r="174" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B174" s="26">
         <v>5</v>
       </c>
       <c r="C174" s="66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D174" s="29"/>
       <c r="E174" s="13"/>
@@ -24848,13 +24857,13 @@
     </row>
     <row r="175" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B175" s="26">
         <v>5</v>
       </c>
       <c r="C175" s="66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="13"/>
@@ -24960,13 +24969,13 @@
     </row>
     <row r="176" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B176" s="26">
         <v>5</v>
       </c>
       <c r="C176" s="66" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="13"/>
@@ -25073,13 +25082,13 @@
     </row>
     <row r="177" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B177" s="26">
         <v>5</v>
       </c>
       <c r="C177" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D177" s="29"/>
       <c r="E177" s="13"/>
@@ -25186,13 +25195,13 @@
     </row>
     <row r="178" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B178" s="26">
         <v>5</v>
       </c>
       <c r="C178" s="55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="13"/>
@@ -25299,13 +25308,13 @@
     </row>
     <row r="179" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B179" s="26">
         <v>5</v>
       </c>
       <c r="C179" s="55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="13"/>
@@ -25412,13 +25421,13 @@
     </row>
     <row r="180" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B180" s="26">
         <v>5</v>
       </c>
       <c r="C180" s="55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D180" s="29"/>
       <c r="E180" s="13"/>
@@ -25525,13 +25534,13 @@
     </row>
     <row r="181" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B181" s="26">
         <v>5</v>
       </c>
       <c r="C181" s="55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="13"/>
@@ -25638,13 +25647,13 @@
     </row>
     <row r="182" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B182" s="26">
         <v>5</v>
       </c>
       <c r="C182" s="55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D182" s="29">
         <v>254</v>
@@ -25856,13 +25865,13 @@
     </row>
     <row r="184" spans="1:323" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B184" s="26">
         <v>3</v>
       </c>
       <c r="C184" s="53" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="13">
@@ -25965,13 +25974,13 @@
     </row>
     <row r="185" spans="1:323" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A185" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B185" s="26">
         <v>3</v>
       </c>
       <c r="C185" s="53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="13">
@@ -26074,13 +26083,13 @@
     </row>
     <row r="186" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B186" s="26">
         <v>3</v>
       </c>
       <c r="C186" s="53" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="13">
@@ -26183,13 +26192,13 @@
     </row>
     <row r="187" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B187" s="26">
         <v>3</v>
       </c>
       <c r="C187" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="13">
@@ -26292,13 +26301,13 @@
     </row>
     <row r="188" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B188" s="26">
         <v>3</v>
       </c>
       <c r="C188" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="13">
@@ -26401,13 +26410,13 @@
     </row>
     <row r="189" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B189" s="26">
         <v>3</v>
       </c>
       <c r="C189" s="53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="13">
@@ -26609,29 +26618,1458 @@
       <c r="LJ190" s="28"/>
       <c r="LK190" s="28"/>
     </row>
-    <row r="191" spans="1:323" x14ac:dyDescent="0.25">
-      <c r="A191" s="14"/>
-      <c r="B191" s="14"/>
+    <row r="191" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="25"/>
+      <c r="B191" s="26"/>
+      <c r="C191" s="53"/>
+      <c r="D191" s="29"/>
+      <c r="E191" s="13"/>
+      <c r="F191" s="13"/>
+      <c r="G191" s="13"/>
+      <c r="H191" s="5"/>
+      <c r="N191" s="28"/>
+      <c r="O191" s="28"/>
+      <c r="U191" s="28"/>
+      <c r="V191" s="28"/>
+      <c r="AB191" s="28"/>
+      <c r="AC191" s="28"/>
+      <c r="AI191" s="28"/>
+      <c r="AJ191" s="28"/>
+      <c r="AP191" s="28"/>
+      <c r="AQ191" s="28"/>
+      <c r="AW191" s="28"/>
+      <c r="AX191" s="28"/>
+      <c r="BD191" s="28"/>
+      <c r="BE191" s="28"/>
+      <c r="BK191" s="28"/>
+      <c r="BL191" s="28"/>
+      <c r="BR191" s="28"/>
+      <c r="BS191" s="28"/>
+      <c r="BY191" s="28"/>
+      <c r="BZ191" s="28"/>
       <c r="CE191" s="38"/>
-      <c r="CG191" s="38"/>
-      <c r="CI191" s="38"/>
-      <c r="CK191" s="38"/>
-    </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C194" s="56"/>
+      <c r="CF191" s="28"/>
+      <c r="CG191" s="28"/>
+      <c r="CM191" s="28"/>
+      <c r="CN191" s="28"/>
+      <c r="CT191" s="28"/>
+      <c r="CU191" s="28"/>
+      <c r="DA191" s="28"/>
+      <c r="DB191" s="28"/>
+      <c r="DH191" s="28"/>
+      <c r="DI191" s="28"/>
+      <c r="DO191" s="28"/>
+      <c r="DP191" s="28"/>
+      <c r="DV191" s="28"/>
+      <c r="DW191" s="28"/>
+      <c r="EC191" s="28"/>
+      <c r="ED191" s="28"/>
+      <c r="EJ191" s="28"/>
+      <c r="EK191" s="28"/>
+      <c r="EQ191" s="28"/>
+      <c r="ER191" s="28"/>
+      <c r="EX191" s="28"/>
+      <c r="EY191" s="28"/>
+      <c r="FE191" s="28"/>
+      <c r="FF191" s="28"/>
+      <c r="FL191" s="28"/>
+      <c r="FM191" s="28"/>
+      <c r="FS191" s="28"/>
+      <c r="FT191" s="28"/>
+      <c r="FZ191" s="28"/>
+      <c r="GA191" s="28"/>
+      <c r="GG191" s="28"/>
+      <c r="GH191" s="28"/>
+      <c r="GN191" s="28"/>
+      <c r="GO191" s="28"/>
+      <c r="GU191" s="28"/>
+      <c r="GV191" s="28"/>
+      <c r="HB191" s="28"/>
+      <c r="HC191" s="28"/>
+      <c r="HI191" s="28"/>
+      <c r="HJ191" s="28"/>
+      <c r="HP191" s="28"/>
+      <c r="HQ191" s="28"/>
+      <c r="HW191" s="28"/>
+      <c r="HX191" s="28"/>
+      <c r="ID191" s="28"/>
+      <c r="IE191" s="28"/>
+      <c r="IK191" s="28"/>
+      <c r="IL191" s="28"/>
+      <c r="IR191" s="28"/>
+      <c r="IS191" s="28"/>
+      <c r="IY191" s="28"/>
+      <c r="IZ191" s="28"/>
+      <c r="JF191" s="28"/>
+      <c r="JG191" s="28"/>
+      <c r="JM191" s="28"/>
+      <c r="JN191" s="28"/>
+      <c r="JT191" s="28"/>
+      <c r="JU191" s="28"/>
+      <c r="KA191" s="28"/>
+      <c r="KB191" s="28"/>
+      <c r="KH191" s="28"/>
+      <c r="KI191" s="28"/>
+      <c r="KO191" s="28"/>
+      <c r="KP191" s="28"/>
+      <c r="KV191" s="28"/>
+      <c r="KW191" s="28"/>
+      <c r="LC191" s="28"/>
+      <c r="LD191" s="28"/>
+      <c r="LJ191" s="28"/>
+      <c r="LK191" s="28"/>
+    </row>
+    <row r="192" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="B192" s="68" t="s">
+        <v>236</v>
+      </c>
+      <c r="C192" s="68"/>
+      <c r="D192" s="29"/>
+      <c r="E192" s="13"/>
+      <c r="F192" s="13"/>
+      <c r="G192" s="13"/>
+      <c r="H192" s="5"/>
+      <c r="N192" s="28"/>
+      <c r="O192" s="28"/>
+      <c r="U192" s="28"/>
+      <c r="V192" s="28"/>
+      <c r="AB192" s="28"/>
+      <c r="AC192" s="28"/>
+      <c r="AI192" s="28"/>
+      <c r="AJ192" s="28"/>
+      <c r="AP192" s="28"/>
+      <c r="AQ192" s="28"/>
+      <c r="AW192" s="28"/>
+      <c r="AX192" s="28"/>
+      <c r="BD192" s="28"/>
+      <c r="BE192" s="28"/>
+      <c r="BK192" s="28"/>
+      <c r="BL192" s="28"/>
+      <c r="BR192" s="28"/>
+      <c r="BS192" s="28"/>
+      <c r="BY192" s="28"/>
+      <c r="BZ192" s="28"/>
+      <c r="CE192" s="38"/>
+      <c r="CF192" s="28"/>
+      <c r="CG192" s="28"/>
+      <c r="CM192" s="28"/>
+      <c r="CN192" s="28"/>
+      <c r="CT192" s="28"/>
+      <c r="CU192" s="28"/>
+      <c r="DA192" s="28"/>
+      <c r="DB192" s="28"/>
+      <c r="DH192" s="28"/>
+      <c r="DI192" s="28"/>
+      <c r="DO192" s="28"/>
+      <c r="DP192" s="28"/>
+      <c r="DV192" s="28"/>
+      <c r="DW192" s="28"/>
+      <c r="EC192" s="28"/>
+      <c r="ED192" s="28"/>
+      <c r="EJ192" s="28"/>
+      <c r="EK192" s="28"/>
+      <c r="EQ192" s="28"/>
+      <c r="ER192" s="28"/>
+      <c r="EX192" s="28"/>
+      <c r="EY192" s="28"/>
+      <c r="FE192" s="28"/>
+      <c r="FF192" s="28"/>
+      <c r="FL192" s="28"/>
+      <c r="FM192" s="28"/>
+      <c r="FS192" s="28"/>
+      <c r="FT192" s="28"/>
+      <c r="FZ192" s="28"/>
+      <c r="GA192" s="28"/>
+      <c r="GG192" s="28"/>
+      <c r="GH192" s="28"/>
+      <c r="GN192" s="28"/>
+      <c r="GO192" s="28"/>
+      <c r="GU192" s="28"/>
+      <c r="GV192" s="28"/>
+      <c r="HB192" s="28"/>
+      <c r="HC192" s="28"/>
+      <c r="HI192" s="28"/>
+      <c r="HJ192" s="28"/>
+      <c r="HP192" s="28"/>
+      <c r="HQ192" s="28"/>
+      <c r="HW192" s="28"/>
+      <c r="HX192" s="28"/>
+      <c r="ID192" s="28"/>
+      <c r="IE192" s="28"/>
+      <c r="IK192" s="28"/>
+      <c r="IL192" s="28"/>
+      <c r="IR192" s="28"/>
+      <c r="IS192" s="28"/>
+      <c r="IY192" s="28"/>
+      <c r="IZ192" s="28"/>
+      <c r="JF192" s="28"/>
+      <c r="JG192" s="28"/>
+      <c r="JM192" s="28"/>
+      <c r="JN192" s="28"/>
+      <c r="JT192" s="28"/>
+      <c r="JU192" s="28"/>
+      <c r="KA192" s="28"/>
+      <c r="KB192" s="28"/>
+      <c r="KH192" s="28"/>
+      <c r="KI192" s="28"/>
+      <c r="KO192" s="28"/>
+      <c r="KP192" s="28"/>
+      <c r="KV192" s="28"/>
+      <c r="KW192" s="28"/>
+      <c r="LC192" s="28"/>
+      <c r="LD192" s="28"/>
+      <c r="LJ192" s="28"/>
+      <c r="LK192" s="28"/>
+    </row>
+    <row r="193" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B193" s="26"/>
+      <c r="C193" s="55" t="s">
+        <v>239</v>
+      </c>
+      <c r="D193" s="29"/>
+      <c r="E193" s="13"/>
+      <c r="F193" s="13">
+        <v>267</v>
+      </c>
+      <c r="G193" s="13">
+        <v>2</v>
+      </c>
+      <c r="H193" s="5">
+        <v>1</v>
+      </c>
+      <c r="N193" s="28"/>
+      <c r="O193" s="28"/>
+      <c r="U193" s="28"/>
+      <c r="V193" s="28"/>
+      <c r="AB193" s="28"/>
+      <c r="AC193" s="28"/>
+      <c r="AI193" s="28"/>
+      <c r="AJ193" s="28"/>
+      <c r="AP193" s="28"/>
+      <c r="AQ193" s="28"/>
+      <c r="AW193" s="28"/>
+      <c r="AX193" s="28"/>
+      <c r="BD193" s="28"/>
+      <c r="BE193" s="28"/>
+      <c r="BK193" s="28"/>
+      <c r="BL193" s="28"/>
+      <c r="BR193" s="28"/>
+      <c r="BS193" s="28"/>
+      <c r="BY193" s="28"/>
+      <c r="BZ193" s="28"/>
+      <c r="CE193" s="38"/>
+      <c r="CF193" s="28"/>
+      <c r="CG193" s="28"/>
+      <c r="CM193" s="28"/>
+      <c r="CN193" s="28"/>
+      <c r="CT193" s="28"/>
+      <c r="CU193" s="28"/>
+      <c r="DA193" s="28"/>
+      <c r="DB193" s="28"/>
+      <c r="DH193" s="28"/>
+      <c r="DI193" s="28"/>
+      <c r="DO193" s="28"/>
+      <c r="DP193" s="28"/>
+      <c r="DV193" s="28"/>
+      <c r="DW193" s="28"/>
+      <c r="EC193" s="28"/>
+      <c r="ED193" s="28"/>
+      <c r="EJ193" s="28"/>
+      <c r="EK193" s="28"/>
+      <c r="EQ193" s="28"/>
+      <c r="ER193" s="28"/>
+      <c r="EX193" s="28"/>
+      <c r="EY193" s="28"/>
+      <c r="FE193" s="28"/>
+      <c r="FF193" s="28"/>
+      <c r="FL193" s="28"/>
+      <c r="FM193" s="28"/>
+      <c r="FS193" s="28"/>
+      <c r="FT193" s="28"/>
+      <c r="FZ193" s="28"/>
+      <c r="GA193" s="28"/>
+      <c r="GG193" s="28"/>
+      <c r="GH193" s="28"/>
+      <c r="GN193" s="28"/>
+      <c r="GO193" s="28"/>
+      <c r="GU193" s="28"/>
+      <c r="GV193" s="28"/>
+      <c r="HB193" s="28"/>
+      <c r="HC193" s="28"/>
+      <c r="HI193" s="28"/>
+      <c r="HJ193" s="28"/>
+      <c r="HP193" s="28"/>
+      <c r="HQ193" s="28"/>
+      <c r="HW193" s="28"/>
+      <c r="HX193" s="28"/>
+      <c r="ID193" s="28"/>
+      <c r="IE193" s="28"/>
+      <c r="IK193" s="28"/>
+      <c r="IL193" s="28"/>
+      <c r="IR193" s="28"/>
+      <c r="IS193" s="28"/>
+      <c r="IY193" s="28"/>
+      <c r="IZ193" s="28"/>
+      <c r="JF193" s="28"/>
+      <c r="JG193" s="28"/>
+      <c r="JM193" s="28"/>
+      <c r="JN193" s="28"/>
+      <c r="JT193" s="28"/>
+      <c r="JU193" s="28"/>
+      <c r="KA193" s="28"/>
+      <c r="KB193" s="28"/>
+      <c r="KH193" s="28"/>
+      <c r="KI193" s="28"/>
+      <c r="KO193" s="28"/>
+      <c r="KP193" s="28"/>
+      <c r="KV193" s="28"/>
+      <c r="KW193" s="28"/>
+      <c r="LC193" s="28"/>
+      <c r="LD193" s="28"/>
+      <c r="LJ193" s="28"/>
+      <c r="LK193" s="28"/>
+    </row>
+    <row r="194" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="25"/>
+      <c r="B194" s="26"/>
+      <c r="C194" s="53"/>
+      <c r="D194" s="29"/>
+      <c r="E194" s="13"/>
+      <c r="F194" s="13"/>
+      <c r="G194" s="13"/>
+      <c r="H194" s="5"/>
+      <c r="N194" s="28"/>
+      <c r="O194" s="28"/>
+      <c r="U194" s="28"/>
+      <c r="V194" s="28"/>
+      <c r="AB194" s="28"/>
+      <c r="AC194" s="28"/>
+      <c r="AI194" s="28"/>
+      <c r="AJ194" s="28"/>
+      <c r="AP194" s="28"/>
+      <c r="AQ194" s="28"/>
+      <c r="AW194" s="28"/>
+      <c r="AX194" s="28"/>
+      <c r="BD194" s="28"/>
+      <c r="BE194" s="28"/>
+      <c r="BK194" s="28"/>
+      <c r="BL194" s="28"/>
+      <c r="BR194" s="28"/>
+      <c r="BS194" s="28"/>
+      <c r="BY194" s="28"/>
+      <c r="BZ194" s="28"/>
+      <c r="CE194" s="38"/>
+      <c r="CF194" s="28"/>
+      <c r="CG194" s="28"/>
+      <c r="CM194" s="28"/>
+      <c r="CN194" s="28"/>
+      <c r="CT194" s="28"/>
+      <c r="CU194" s="28"/>
+      <c r="DA194" s="28"/>
+      <c r="DB194" s="28"/>
+      <c r="DH194" s="28"/>
+      <c r="DI194" s="28"/>
+      <c r="DO194" s="28"/>
+      <c r="DP194" s="28"/>
+      <c r="DV194" s="28"/>
+      <c r="DW194" s="28"/>
+      <c r="EC194" s="28"/>
+      <c r="ED194" s="28"/>
+      <c r="EJ194" s="28"/>
+      <c r="EK194" s="28"/>
+      <c r="EQ194" s="28"/>
+      <c r="ER194" s="28"/>
+      <c r="EX194" s="28"/>
+      <c r="EY194" s="28"/>
+      <c r="FE194" s="28"/>
+      <c r="FF194" s="28"/>
+      <c r="FL194" s="28"/>
+      <c r="FM194" s="28"/>
+      <c r="FS194" s="28"/>
+      <c r="FT194" s="28"/>
+      <c r="FZ194" s="28"/>
+      <c r="GA194" s="28"/>
+      <c r="GG194" s="28"/>
+      <c r="GH194" s="28"/>
+      <c r="GN194" s="28"/>
+      <c r="GO194" s="28"/>
+      <c r="GU194" s="28"/>
+      <c r="GV194" s="28"/>
+      <c r="HB194" s="28"/>
+      <c r="HC194" s="28"/>
+      <c r="HI194" s="28"/>
+      <c r="HJ194" s="28"/>
+      <c r="HP194" s="28"/>
+      <c r="HQ194" s="28"/>
+      <c r="HW194" s="28"/>
+      <c r="HX194" s="28"/>
+      <c r="ID194" s="28"/>
+      <c r="IE194" s="28"/>
+      <c r="IK194" s="28"/>
+      <c r="IL194" s="28"/>
+      <c r="IR194" s="28"/>
+      <c r="IS194" s="28"/>
+      <c r="IY194" s="28"/>
+      <c r="IZ194" s="28"/>
+      <c r="JF194" s="28"/>
+      <c r="JG194" s="28"/>
+      <c r="JM194" s="28"/>
+      <c r="JN194" s="28"/>
+      <c r="JT194" s="28"/>
+      <c r="JU194" s="28"/>
+      <c r="KA194" s="28"/>
+      <c r="KB194" s="28"/>
+      <c r="KH194" s="28"/>
+      <c r="KI194" s="28"/>
+      <c r="KO194" s="28"/>
+      <c r="KP194" s="28"/>
+      <c r="KV194" s="28"/>
+      <c r="KW194" s="28"/>
+      <c r="LC194" s="28"/>
+      <c r="LD194" s="28"/>
+      <c r="LJ194" s="28"/>
+      <c r="LK194" s="28"/>
+    </row>
+    <row r="195" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="25"/>
+      <c r="B195" s="26"/>
+      <c r="C195" s="53"/>
+      <c r="D195" s="29"/>
+      <c r="E195" s="13"/>
+      <c r="F195" s="13"/>
+      <c r="G195" s="13"/>
+      <c r="H195" s="5"/>
+      <c r="N195" s="28"/>
+      <c r="O195" s="28"/>
+      <c r="U195" s="28"/>
+      <c r="V195" s="28"/>
+      <c r="AB195" s="28"/>
+      <c r="AC195" s="28"/>
+      <c r="AI195" s="28"/>
+      <c r="AJ195" s="28"/>
+      <c r="AP195" s="28"/>
+      <c r="AQ195" s="28"/>
+      <c r="AW195" s="28"/>
+      <c r="AX195" s="28"/>
+      <c r="BD195" s="28"/>
+      <c r="BE195" s="28"/>
+      <c r="BK195" s="28"/>
+      <c r="BL195" s="28"/>
+      <c r="BR195" s="28"/>
+      <c r="BS195" s="28"/>
+      <c r="BY195" s="28"/>
+      <c r="BZ195" s="28"/>
+      <c r="CE195" s="38"/>
+      <c r="CF195" s="28"/>
+      <c r="CG195" s="28"/>
+      <c r="CM195" s="28"/>
+      <c r="CN195" s="28"/>
+      <c r="CT195" s="28"/>
+      <c r="CU195" s="28"/>
+      <c r="DA195" s="28"/>
+      <c r="DB195" s="28"/>
+      <c r="DH195" s="28"/>
+      <c r="DI195" s="28"/>
+      <c r="DO195" s="28"/>
+      <c r="DP195" s="28"/>
+      <c r="DV195" s="28"/>
+      <c r="DW195" s="28"/>
+      <c r="EC195" s="28"/>
+      <c r="ED195" s="28"/>
+      <c r="EJ195" s="28"/>
+      <c r="EK195" s="28"/>
+      <c r="EQ195" s="28"/>
+      <c r="ER195" s="28"/>
+      <c r="EX195" s="28"/>
+      <c r="EY195" s="28"/>
+      <c r="FE195" s="28"/>
+      <c r="FF195" s="28"/>
+      <c r="FL195" s="28"/>
+      <c r="FM195" s="28"/>
+      <c r="FS195" s="28"/>
+      <c r="FT195" s="28"/>
+      <c r="FZ195" s="28"/>
+      <c r="GA195" s="28"/>
+      <c r="GG195" s="28"/>
+      <c r="GH195" s="28"/>
+      <c r="GN195" s="28"/>
+      <c r="GO195" s="28"/>
+      <c r="GU195" s="28"/>
+      <c r="GV195" s="28"/>
+      <c r="HB195" s="28"/>
+      <c r="HC195" s="28"/>
+      <c r="HI195" s="28"/>
+      <c r="HJ195" s="28"/>
+      <c r="HP195" s="28"/>
+      <c r="HQ195" s="28"/>
+      <c r="HW195" s="28"/>
+      <c r="HX195" s="28"/>
+      <c r="ID195" s="28"/>
+      <c r="IE195" s="28"/>
+      <c r="IK195" s="28"/>
+      <c r="IL195" s="28"/>
+      <c r="IR195" s="28"/>
+      <c r="IS195" s="28"/>
+      <c r="IY195" s="28"/>
+      <c r="IZ195" s="28"/>
+      <c r="JF195" s="28"/>
+      <c r="JG195" s="28"/>
+      <c r="JM195" s="28"/>
+      <c r="JN195" s="28"/>
+      <c r="JT195" s="28"/>
+      <c r="JU195" s="28"/>
+      <c r="KA195" s="28"/>
+      <c r="KB195" s="28"/>
+      <c r="KH195" s="28"/>
+      <c r="KI195" s="28"/>
+      <c r="KO195" s="28"/>
+      <c r="KP195" s="28"/>
+      <c r="KV195" s="28"/>
+      <c r="KW195" s="28"/>
+      <c r="LC195" s="28"/>
+      <c r="LD195" s="28"/>
+      <c r="LJ195" s="28"/>
+      <c r="LK195" s="28"/>
+    </row>
+    <row r="196" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="25"/>
+      <c r="B196" s="26"/>
+      <c r="C196" s="53"/>
+      <c r="D196" s="29"/>
+      <c r="E196" s="13"/>
+      <c r="F196" s="13"/>
+      <c r="G196" s="13"/>
+      <c r="H196" s="5"/>
+      <c r="N196" s="28"/>
+      <c r="O196" s="28"/>
+      <c r="U196" s="28"/>
+      <c r="V196" s="28"/>
+      <c r="AB196" s="28"/>
+      <c r="AC196" s="28"/>
+      <c r="AI196" s="28"/>
+      <c r="AJ196" s="28"/>
+      <c r="AP196" s="28"/>
+      <c r="AQ196" s="28"/>
+      <c r="AW196" s="28"/>
+      <c r="AX196" s="28"/>
+      <c r="BD196" s="28"/>
+      <c r="BE196" s="28"/>
+      <c r="BK196" s="28"/>
+      <c r="BL196" s="28"/>
+      <c r="BR196" s="28"/>
+      <c r="BS196" s="28"/>
+      <c r="BY196" s="28"/>
+      <c r="BZ196" s="28"/>
+      <c r="CE196" s="38"/>
+      <c r="CF196" s="28"/>
+      <c r="CG196" s="28"/>
+      <c r="CM196" s="28"/>
+      <c r="CN196" s="28"/>
+      <c r="CT196" s="28"/>
+      <c r="CU196" s="28"/>
+      <c r="DA196" s="28"/>
+      <c r="DB196" s="28"/>
+      <c r="DH196" s="28"/>
+      <c r="DI196" s="28"/>
+      <c r="DO196" s="28"/>
+      <c r="DP196" s="28"/>
+      <c r="DV196" s="28"/>
+      <c r="DW196" s="28"/>
+      <c r="EC196" s="28"/>
+      <c r="ED196" s="28"/>
+      <c r="EJ196" s="28"/>
+      <c r="EK196" s="28"/>
+      <c r="EQ196" s="28"/>
+      <c r="ER196" s="28"/>
+      <c r="EX196" s="28"/>
+      <c r="EY196" s="28"/>
+      <c r="FE196" s="28"/>
+      <c r="FF196" s="28"/>
+      <c r="FL196" s="28"/>
+      <c r="FM196" s="28"/>
+      <c r="FS196" s="28"/>
+      <c r="FT196" s="28"/>
+      <c r="FZ196" s="28"/>
+      <c r="GA196" s="28"/>
+      <c r="GG196" s="28"/>
+      <c r="GH196" s="28"/>
+      <c r="GN196" s="28"/>
+      <c r="GO196" s="28"/>
+      <c r="GU196" s="28"/>
+      <c r="GV196" s="28"/>
+      <c r="HB196" s="28"/>
+      <c r="HC196" s="28"/>
+      <c r="HI196" s="28"/>
+      <c r="HJ196" s="28"/>
+      <c r="HP196" s="28"/>
+      <c r="HQ196" s="28"/>
+      <c r="HW196" s="28"/>
+      <c r="HX196" s="28"/>
+      <c r="ID196" s="28"/>
+      <c r="IE196" s="28"/>
+      <c r="IK196" s="28"/>
+      <c r="IL196" s="28"/>
+      <c r="IR196" s="28"/>
+      <c r="IS196" s="28"/>
+      <c r="IY196" s="28"/>
+      <c r="IZ196" s="28"/>
+      <c r="JF196" s="28"/>
+      <c r="JG196" s="28"/>
+      <c r="JM196" s="28"/>
+      <c r="JN196" s="28"/>
+      <c r="JT196" s="28"/>
+      <c r="JU196" s="28"/>
+      <c r="KA196" s="28"/>
+      <c r="KB196" s="28"/>
+      <c r="KH196" s="28"/>
+      <c r="KI196" s="28"/>
+      <c r="KO196" s="28"/>
+      <c r="KP196" s="28"/>
+      <c r="KV196" s="28"/>
+      <c r="KW196" s="28"/>
+      <c r="LC196" s="28"/>
+      <c r="LD196" s="28"/>
+      <c r="LJ196" s="28"/>
+      <c r="LK196" s="28"/>
+    </row>
+    <row r="197" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="25"/>
+      <c r="B197" s="26"/>
+      <c r="C197" s="53"/>
+      <c r="D197" s="29"/>
+      <c r="E197" s="13"/>
+      <c r="F197" s="13"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="5"/>
+      <c r="N197" s="28"/>
+      <c r="O197" s="28"/>
+      <c r="U197" s="28"/>
+      <c r="V197" s="28"/>
+      <c r="AB197" s="28"/>
+      <c r="AC197" s="28"/>
+      <c r="AI197" s="28"/>
+      <c r="AJ197" s="28"/>
+      <c r="AP197" s="28"/>
+      <c r="AQ197" s="28"/>
+      <c r="AW197" s="28"/>
+      <c r="AX197" s="28"/>
+      <c r="BD197" s="28"/>
+      <c r="BE197" s="28"/>
+      <c r="BK197" s="28"/>
+      <c r="BL197" s="28"/>
+      <c r="BR197" s="28"/>
+      <c r="BS197" s="28"/>
+      <c r="BY197" s="28"/>
+      <c r="BZ197" s="28"/>
+      <c r="CE197" s="38"/>
+      <c r="CF197" s="28"/>
+      <c r="CG197" s="28"/>
+      <c r="CM197" s="28"/>
+      <c r="CN197" s="28"/>
+      <c r="CT197" s="28"/>
+      <c r="CU197" s="28"/>
+      <c r="DA197" s="28"/>
+      <c r="DB197" s="28"/>
+      <c r="DH197" s="28"/>
+      <c r="DI197" s="28"/>
+      <c r="DO197" s="28"/>
+      <c r="DP197" s="28"/>
+      <c r="DV197" s="28"/>
+      <c r="DW197" s="28"/>
+      <c r="EC197" s="28"/>
+      <c r="ED197" s="28"/>
+      <c r="EJ197" s="28"/>
+      <c r="EK197" s="28"/>
+      <c r="EQ197" s="28"/>
+      <c r="ER197" s="28"/>
+      <c r="EX197" s="28"/>
+      <c r="EY197" s="28"/>
+      <c r="FE197" s="28"/>
+      <c r="FF197" s="28"/>
+      <c r="FL197" s="28"/>
+      <c r="FM197" s="28"/>
+      <c r="FS197" s="28"/>
+      <c r="FT197" s="28"/>
+      <c r="FZ197" s="28"/>
+      <c r="GA197" s="28"/>
+      <c r="GG197" s="28"/>
+      <c r="GH197" s="28"/>
+      <c r="GN197" s="28"/>
+      <c r="GO197" s="28"/>
+      <c r="GU197" s="28"/>
+      <c r="GV197" s="28"/>
+      <c r="HB197" s="28"/>
+      <c r="HC197" s="28"/>
+      <c r="HI197" s="28"/>
+      <c r="HJ197" s="28"/>
+      <c r="HP197" s="28"/>
+      <c r="HQ197" s="28"/>
+      <c r="HW197" s="28"/>
+      <c r="HX197" s="28"/>
+      <c r="ID197" s="28"/>
+      <c r="IE197" s="28"/>
+      <c r="IK197" s="28"/>
+      <c r="IL197" s="28"/>
+      <c r="IR197" s="28"/>
+      <c r="IS197" s="28"/>
+      <c r="IY197" s="28"/>
+      <c r="IZ197" s="28"/>
+      <c r="JF197" s="28"/>
+      <c r="JG197" s="28"/>
+      <c r="JM197" s="28"/>
+      <c r="JN197" s="28"/>
+      <c r="JT197" s="28"/>
+      <c r="JU197" s="28"/>
+      <c r="KA197" s="28"/>
+      <c r="KB197" s="28"/>
+      <c r="KH197" s="28"/>
+      <c r="KI197" s="28"/>
+      <c r="KO197" s="28"/>
+      <c r="KP197" s="28"/>
+      <c r="KV197" s="28"/>
+      <c r="KW197" s="28"/>
+      <c r="LC197" s="28"/>
+      <c r="LD197" s="28"/>
+      <c r="LJ197" s="28"/>
+      <c r="LK197" s="28"/>
+    </row>
+    <row r="198" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="25"/>
+      <c r="B198" s="26"/>
+      <c r="C198" s="53"/>
+      <c r="D198" s="29"/>
+      <c r="E198" s="13"/>
+      <c r="F198" s="13"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="5"/>
+      <c r="N198" s="28"/>
+      <c r="O198" s="28"/>
+      <c r="U198" s="28"/>
+      <c r="V198" s="28"/>
+      <c r="AB198" s="28"/>
+      <c r="AC198" s="28"/>
+      <c r="AI198" s="28"/>
+      <c r="AJ198" s="28"/>
+      <c r="AP198" s="28"/>
+      <c r="AQ198" s="28"/>
+      <c r="AW198" s="28"/>
+      <c r="AX198" s="28"/>
+      <c r="BD198" s="28"/>
+      <c r="BE198" s="28"/>
+      <c r="BK198" s="28"/>
+      <c r="BL198" s="28"/>
+      <c r="BR198" s="28"/>
+      <c r="BS198" s="28"/>
+      <c r="BY198" s="28"/>
+      <c r="BZ198" s="28"/>
+      <c r="CE198" s="38"/>
+      <c r="CF198" s="28"/>
+      <c r="CG198" s="28"/>
+      <c r="CM198" s="28"/>
+      <c r="CN198" s="28"/>
+      <c r="CT198" s="28"/>
+      <c r="CU198" s="28"/>
+      <c r="DA198" s="28"/>
+      <c r="DB198" s="28"/>
+      <c r="DH198" s="28"/>
+      <c r="DI198" s="28"/>
+      <c r="DO198" s="28"/>
+      <c r="DP198" s="28"/>
+      <c r="DV198" s="28"/>
+      <c r="DW198" s="28"/>
+      <c r="EC198" s="28"/>
+      <c r="ED198" s="28"/>
+      <c r="EJ198" s="28"/>
+      <c r="EK198" s="28"/>
+      <c r="EQ198" s="28"/>
+      <c r="ER198" s="28"/>
+      <c r="EX198" s="28"/>
+      <c r="EY198" s="28"/>
+      <c r="FE198" s="28"/>
+      <c r="FF198" s="28"/>
+      <c r="FL198" s="28"/>
+      <c r="FM198" s="28"/>
+      <c r="FS198" s="28"/>
+      <c r="FT198" s="28"/>
+      <c r="FZ198" s="28"/>
+      <c r="GA198" s="28"/>
+      <c r="GG198" s="28"/>
+      <c r="GH198" s="28"/>
+      <c r="GN198" s="28"/>
+      <c r="GO198" s="28"/>
+      <c r="GU198" s="28"/>
+      <c r="GV198" s="28"/>
+      <c r="HB198" s="28"/>
+      <c r="HC198" s="28"/>
+      <c r="HI198" s="28"/>
+      <c r="HJ198" s="28"/>
+      <c r="HP198" s="28"/>
+      <c r="HQ198" s="28"/>
+      <c r="HW198" s="28"/>
+      <c r="HX198" s="28"/>
+      <c r="ID198" s="28"/>
+      <c r="IE198" s="28"/>
+      <c r="IK198" s="28"/>
+      <c r="IL198" s="28"/>
+      <c r="IR198" s="28"/>
+      <c r="IS198" s="28"/>
+      <c r="IY198" s="28"/>
+      <c r="IZ198" s="28"/>
+      <c r="JF198" s="28"/>
+      <c r="JG198" s="28"/>
+      <c r="JM198" s="28"/>
+      <c r="JN198" s="28"/>
+      <c r="JT198" s="28"/>
+      <c r="JU198" s="28"/>
+      <c r="KA198" s="28"/>
+      <c r="KB198" s="28"/>
+      <c r="KH198" s="28"/>
+      <c r="KI198" s="28"/>
+      <c r="KO198" s="28"/>
+      <c r="KP198" s="28"/>
+      <c r="KV198" s="28"/>
+      <c r="KW198" s="28"/>
+      <c r="LC198" s="28"/>
+      <c r="LD198" s="28"/>
+      <c r="LJ198" s="28"/>
+      <c r="LK198" s="28"/>
+    </row>
+    <row r="199" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="25"/>
+      <c r="B199" s="26"/>
+      <c r="C199" s="53"/>
+      <c r="D199" s="29"/>
+      <c r="E199" s="13"/>
+      <c r="F199" s="13"/>
+      <c r="G199" s="13"/>
+      <c r="H199" s="5"/>
+      <c r="N199" s="28"/>
+      <c r="O199" s="28"/>
+      <c r="U199" s="28"/>
+      <c r="V199" s="28"/>
+      <c r="AB199" s="28"/>
+      <c r="AC199" s="28"/>
+      <c r="AI199" s="28"/>
+      <c r="AJ199" s="28"/>
+      <c r="AP199" s="28"/>
+      <c r="AQ199" s="28"/>
+      <c r="AW199" s="28"/>
+      <c r="AX199" s="28"/>
+      <c r="BD199" s="28"/>
+      <c r="BE199" s="28"/>
+      <c r="BK199" s="28"/>
+      <c r="BL199" s="28"/>
+      <c r="BR199" s="28"/>
+      <c r="BS199" s="28"/>
+      <c r="BY199" s="28"/>
+      <c r="BZ199" s="28"/>
+      <c r="CE199" s="38"/>
+      <c r="CF199" s="28"/>
+      <c r="CG199" s="28"/>
+      <c r="CM199" s="28"/>
+      <c r="CN199" s="28"/>
+      <c r="CT199" s="28"/>
+      <c r="CU199" s="28"/>
+      <c r="DA199" s="28"/>
+      <c r="DB199" s="28"/>
+      <c r="DH199" s="28"/>
+      <c r="DI199" s="28"/>
+      <c r="DO199" s="28"/>
+      <c r="DP199" s="28"/>
+      <c r="DV199" s="28"/>
+      <c r="DW199" s="28"/>
+      <c r="EC199" s="28"/>
+      <c r="ED199" s="28"/>
+      <c r="EJ199" s="28"/>
+      <c r="EK199" s="28"/>
+      <c r="EQ199" s="28"/>
+      <c r="ER199" s="28"/>
+      <c r="EX199" s="28"/>
+      <c r="EY199" s="28"/>
+      <c r="FE199" s="28"/>
+      <c r="FF199" s="28"/>
+      <c r="FL199" s="28"/>
+      <c r="FM199" s="28"/>
+      <c r="FS199" s="28"/>
+      <c r="FT199" s="28"/>
+      <c r="FZ199" s="28"/>
+      <c r="GA199" s="28"/>
+      <c r="GG199" s="28"/>
+      <c r="GH199" s="28"/>
+      <c r="GN199" s="28"/>
+      <c r="GO199" s="28"/>
+      <c r="GU199" s="28"/>
+      <c r="GV199" s="28"/>
+      <c r="HB199" s="28"/>
+      <c r="HC199" s="28"/>
+      <c r="HI199" s="28"/>
+      <c r="HJ199" s="28"/>
+      <c r="HP199" s="28"/>
+      <c r="HQ199" s="28"/>
+      <c r="HW199" s="28"/>
+      <c r="HX199" s="28"/>
+      <c r="ID199" s="28"/>
+      <c r="IE199" s="28"/>
+      <c r="IK199" s="28"/>
+      <c r="IL199" s="28"/>
+      <c r="IR199" s="28"/>
+      <c r="IS199" s="28"/>
+      <c r="IY199" s="28"/>
+      <c r="IZ199" s="28"/>
+      <c r="JF199" s="28"/>
+      <c r="JG199" s="28"/>
+      <c r="JM199" s="28"/>
+      <c r="JN199" s="28"/>
+      <c r="JT199" s="28"/>
+      <c r="JU199" s="28"/>
+      <c r="KA199" s="28"/>
+      <c r="KB199" s="28"/>
+      <c r="KH199" s="28"/>
+      <c r="KI199" s="28"/>
+      <c r="KO199" s="28"/>
+      <c r="KP199" s="28"/>
+      <c r="KV199" s="28"/>
+      <c r="KW199" s="28"/>
+      <c r="LC199" s="28"/>
+      <c r="LD199" s="28"/>
+      <c r="LJ199" s="28"/>
+      <c r="LK199" s="28"/>
+    </row>
+    <row r="200" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="25"/>
+      <c r="B200" s="26"/>
+      <c r="C200" s="53"/>
+      <c r="D200" s="29"/>
+      <c r="E200" s="13"/>
+      <c r="F200" s="13"/>
+      <c r="G200" s="13"/>
+      <c r="H200" s="5"/>
+      <c r="N200" s="28"/>
+      <c r="O200" s="28"/>
+      <c r="U200" s="28"/>
+      <c r="V200" s="28"/>
+      <c r="AB200" s="28"/>
+      <c r="AC200" s="28"/>
+      <c r="AI200" s="28"/>
+      <c r="AJ200" s="28"/>
+      <c r="AP200" s="28"/>
+      <c r="AQ200" s="28"/>
+      <c r="AW200" s="28"/>
+      <c r="AX200" s="28"/>
+      <c r="BD200" s="28"/>
+      <c r="BE200" s="28"/>
+      <c r="BK200" s="28"/>
+      <c r="BL200" s="28"/>
+      <c r="BR200" s="28"/>
+      <c r="BS200" s="28"/>
+      <c r="BY200" s="28"/>
+      <c r="BZ200" s="28"/>
+      <c r="CE200" s="38"/>
+      <c r="CF200" s="28"/>
+      <c r="CG200" s="28"/>
+      <c r="CM200" s="28"/>
+      <c r="CN200" s="28"/>
+      <c r="CT200" s="28"/>
+      <c r="CU200" s="28"/>
+      <c r="DA200" s="28"/>
+      <c r="DB200" s="28"/>
+      <c r="DH200" s="28"/>
+      <c r="DI200" s="28"/>
+      <c r="DO200" s="28"/>
+      <c r="DP200" s="28"/>
+      <c r="DV200" s="28"/>
+      <c r="DW200" s="28"/>
+      <c r="EC200" s="28"/>
+      <c r="ED200" s="28"/>
+      <c r="EJ200" s="28"/>
+      <c r="EK200" s="28"/>
+      <c r="EQ200" s="28"/>
+      <c r="ER200" s="28"/>
+      <c r="EX200" s="28"/>
+      <c r="EY200" s="28"/>
+      <c r="FE200" s="28"/>
+      <c r="FF200" s="28"/>
+      <c r="FL200" s="28"/>
+      <c r="FM200" s="28"/>
+      <c r="FS200" s="28"/>
+      <c r="FT200" s="28"/>
+      <c r="FZ200" s="28"/>
+      <c r="GA200" s="28"/>
+      <c r="GG200" s="28"/>
+      <c r="GH200" s="28"/>
+      <c r="GN200" s="28"/>
+      <c r="GO200" s="28"/>
+      <c r="GU200" s="28"/>
+      <c r="GV200" s="28"/>
+      <c r="HB200" s="28"/>
+      <c r="HC200" s="28"/>
+      <c r="HI200" s="28"/>
+      <c r="HJ200" s="28"/>
+      <c r="HP200" s="28"/>
+      <c r="HQ200" s="28"/>
+      <c r="HW200" s="28"/>
+      <c r="HX200" s="28"/>
+      <c r="ID200" s="28"/>
+      <c r="IE200" s="28"/>
+      <c r="IK200" s="28"/>
+      <c r="IL200" s="28"/>
+      <c r="IR200" s="28"/>
+      <c r="IS200" s="28"/>
+      <c r="IY200" s="28"/>
+      <c r="IZ200" s="28"/>
+      <c r="JF200" s="28"/>
+      <c r="JG200" s="28"/>
+      <c r="JM200" s="28"/>
+      <c r="JN200" s="28"/>
+      <c r="JT200" s="28"/>
+      <c r="JU200" s="28"/>
+      <c r="KA200" s="28"/>
+      <c r="KB200" s="28"/>
+      <c r="KH200" s="28"/>
+      <c r="KI200" s="28"/>
+      <c r="KO200" s="28"/>
+      <c r="KP200" s="28"/>
+      <c r="KV200" s="28"/>
+      <c r="KW200" s="28"/>
+      <c r="LC200" s="28"/>
+      <c r="LD200" s="28"/>
+      <c r="LJ200" s="28"/>
+      <c r="LK200" s="28"/>
+    </row>
+    <row r="201" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="25"/>
+      <c r="B201" s="26"/>
+      <c r="C201" s="53"/>
+      <c r="D201" s="29"/>
+      <c r="E201" s="13"/>
+      <c r="F201" s="13"/>
+      <c r="G201" s="13"/>
+      <c r="H201" s="5"/>
+      <c r="N201" s="28"/>
+      <c r="O201" s="28"/>
+      <c r="U201" s="28"/>
+      <c r="V201" s="28"/>
+      <c r="AB201" s="28"/>
+      <c r="AC201" s="28"/>
+      <c r="AI201" s="28"/>
+      <c r="AJ201" s="28"/>
+      <c r="AP201" s="28"/>
+      <c r="AQ201" s="28"/>
+      <c r="AW201" s="28"/>
+      <c r="AX201" s="28"/>
+      <c r="BD201" s="28"/>
+      <c r="BE201" s="28"/>
+      <c r="BK201" s="28"/>
+      <c r="BL201" s="28"/>
+      <c r="BR201" s="28"/>
+      <c r="BS201" s="28"/>
+      <c r="BY201" s="28"/>
+      <c r="BZ201" s="28"/>
+      <c r="CE201" s="38"/>
+      <c r="CF201" s="28"/>
+      <c r="CG201" s="28"/>
+      <c r="CM201" s="28"/>
+      <c r="CN201" s="28"/>
+      <c r="CT201" s="28"/>
+      <c r="CU201" s="28"/>
+      <c r="DA201" s="28"/>
+      <c r="DB201" s="28"/>
+      <c r="DH201" s="28"/>
+      <c r="DI201" s="28"/>
+      <c r="DO201" s="28"/>
+      <c r="DP201" s="28"/>
+      <c r="DV201" s="28"/>
+      <c r="DW201" s="28"/>
+      <c r="EC201" s="28"/>
+      <c r="ED201" s="28"/>
+      <c r="EJ201" s="28"/>
+      <c r="EK201" s="28"/>
+      <c r="EQ201" s="28"/>
+      <c r="ER201" s="28"/>
+      <c r="EX201" s="28"/>
+      <c r="EY201" s="28"/>
+      <c r="FE201" s="28"/>
+      <c r="FF201" s="28"/>
+      <c r="FL201" s="28"/>
+      <c r="FM201" s="28"/>
+      <c r="FS201" s="28"/>
+      <c r="FT201" s="28"/>
+      <c r="FZ201" s="28"/>
+      <c r="GA201" s="28"/>
+      <c r="GG201" s="28"/>
+      <c r="GH201" s="28"/>
+      <c r="GN201" s="28"/>
+      <c r="GO201" s="28"/>
+      <c r="GU201" s="28"/>
+      <c r="GV201" s="28"/>
+      <c r="HB201" s="28"/>
+      <c r="HC201" s="28"/>
+      <c r="HI201" s="28"/>
+      <c r="HJ201" s="28"/>
+      <c r="HP201" s="28"/>
+      <c r="HQ201" s="28"/>
+      <c r="HW201" s="28"/>
+      <c r="HX201" s="28"/>
+      <c r="ID201" s="28"/>
+      <c r="IE201" s="28"/>
+      <c r="IK201" s="28"/>
+      <c r="IL201" s="28"/>
+      <c r="IR201" s="28"/>
+      <c r="IS201" s="28"/>
+      <c r="IY201" s="28"/>
+      <c r="IZ201" s="28"/>
+      <c r="JF201" s="28"/>
+      <c r="JG201" s="28"/>
+      <c r="JM201" s="28"/>
+      <c r="JN201" s="28"/>
+      <c r="JT201" s="28"/>
+      <c r="JU201" s="28"/>
+      <c r="KA201" s="28"/>
+      <c r="KB201" s="28"/>
+      <c r="KH201" s="28"/>
+      <c r="KI201" s="28"/>
+      <c r="KO201" s="28"/>
+      <c r="KP201" s="28"/>
+      <c r="KV201" s="28"/>
+      <c r="KW201" s="28"/>
+      <c r="LC201" s="28"/>
+      <c r="LD201" s="28"/>
+      <c r="LJ201" s="28"/>
+      <c r="LK201" s="28"/>
+    </row>
+    <row r="202" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="25"/>
+      <c r="B202" s="26"/>
+      <c r="C202" s="53"/>
+      <c r="D202" s="29"/>
+      <c r="E202" s="13"/>
+      <c r="F202" s="13"/>
+      <c r="G202" s="13"/>
+      <c r="H202" s="5"/>
+      <c r="N202" s="28"/>
+      <c r="O202" s="28"/>
+      <c r="U202" s="28"/>
+      <c r="V202" s="28"/>
+      <c r="AB202" s="28"/>
+      <c r="AC202" s="28"/>
+      <c r="AI202" s="28"/>
+      <c r="AJ202" s="28"/>
+      <c r="AP202" s="28"/>
+      <c r="AQ202" s="28"/>
+      <c r="AW202" s="28"/>
+      <c r="AX202" s="28"/>
+      <c r="BD202" s="28"/>
+      <c r="BE202" s="28"/>
+      <c r="BK202" s="28"/>
+      <c r="BL202" s="28"/>
+      <c r="BR202" s="28"/>
+      <c r="BS202" s="28"/>
+      <c r="BY202" s="28"/>
+      <c r="BZ202" s="28"/>
+      <c r="CE202" s="38"/>
+      <c r="CF202" s="28"/>
+      <c r="CG202" s="28"/>
+      <c r="CM202" s="28"/>
+      <c r="CN202" s="28"/>
+      <c r="CT202" s="28"/>
+      <c r="CU202" s="28"/>
+      <c r="DA202" s="28"/>
+      <c r="DB202" s="28"/>
+      <c r="DH202" s="28"/>
+      <c r="DI202" s="28"/>
+      <c r="DO202" s="28"/>
+      <c r="DP202" s="28"/>
+      <c r="DV202" s="28"/>
+      <c r="DW202" s="28"/>
+      <c r="EC202" s="28"/>
+      <c r="ED202" s="28"/>
+      <c r="EJ202" s="28"/>
+      <c r="EK202" s="28"/>
+      <c r="EQ202" s="28"/>
+      <c r="ER202" s="28"/>
+      <c r="EX202" s="28"/>
+      <c r="EY202" s="28"/>
+      <c r="FE202" s="28"/>
+      <c r="FF202" s="28"/>
+      <c r="FL202" s="28"/>
+      <c r="FM202" s="28"/>
+      <c r="FS202" s="28"/>
+      <c r="FT202" s="28"/>
+      <c r="FZ202" s="28"/>
+      <c r="GA202" s="28"/>
+      <c r="GG202" s="28"/>
+      <c r="GH202" s="28"/>
+      <c r="GN202" s="28"/>
+      <c r="GO202" s="28"/>
+      <c r="GU202" s="28"/>
+      <c r="GV202" s="28"/>
+      <c r="HB202" s="28"/>
+      <c r="HC202" s="28"/>
+      <c r="HI202" s="28"/>
+      <c r="HJ202" s="28"/>
+      <c r="HP202" s="28"/>
+      <c r="HQ202" s="28"/>
+      <c r="HW202" s="28"/>
+      <c r="HX202" s="28"/>
+      <c r="ID202" s="28"/>
+      <c r="IE202" s="28"/>
+      <c r="IK202" s="28"/>
+      <c r="IL202" s="28"/>
+      <c r="IR202" s="28"/>
+      <c r="IS202" s="28"/>
+      <c r="IY202" s="28"/>
+      <c r="IZ202" s="28"/>
+      <c r="JF202" s="28"/>
+      <c r="JG202" s="28"/>
+      <c r="JM202" s="28"/>
+      <c r="JN202" s="28"/>
+      <c r="JT202" s="28"/>
+      <c r="JU202" s="28"/>
+      <c r="KA202" s="28"/>
+      <c r="KB202" s="28"/>
+      <c r="KH202" s="28"/>
+      <c r="KI202" s="28"/>
+      <c r="KO202" s="28"/>
+      <c r="KP202" s="28"/>
+      <c r="KV202" s="28"/>
+      <c r="KW202" s="28"/>
+      <c r="LC202" s="28"/>
+      <c r="LD202" s="28"/>
+      <c r="LJ202" s="28"/>
+      <c r="LK202" s="28"/>
+    </row>
+    <row r="203" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="25"/>
+      <c r="B203" s="26"/>
+      <c r="C203" s="53"/>
+      <c r="D203" s="29"/>
+      <c r="E203" s="13"/>
+      <c r="F203" s="13"/>
+      <c r="G203" s="13"/>
+      <c r="H203" s="5"/>
+      <c r="N203" s="28"/>
+      <c r="O203" s="28"/>
+      <c r="U203" s="28"/>
+      <c r="V203" s="28"/>
+      <c r="AB203" s="28"/>
+      <c r="AC203" s="28"/>
+      <c r="AI203" s="28"/>
+      <c r="AJ203" s="28"/>
+      <c r="AP203" s="28"/>
+      <c r="AQ203" s="28"/>
+      <c r="AW203" s="28"/>
+      <c r="AX203" s="28"/>
+      <c r="BD203" s="28"/>
+      <c r="BE203" s="28"/>
+      <c r="BK203" s="28"/>
+      <c r="BL203" s="28"/>
+      <c r="BR203" s="28"/>
+      <c r="BS203" s="28"/>
+      <c r="BY203" s="28"/>
+      <c r="BZ203" s="28"/>
+      <c r="CE203" s="38"/>
+      <c r="CF203" s="28"/>
+      <c r="CG203" s="28"/>
+      <c r="CM203" s="28"/>
+      <c r="CN203" s="28"/>
+      <c r="CT203" s="28"/>
+      <c r="CU203" s="28"/>
+      <c r="DA203" s="28"/>
+      <c r="DB203" s="28"/>
+      <c r="DH203" s="28"/>
+      <c r="DI203" s="28"/>
+      <c r="DO203" s="28"/>
+      <c r="DP203" s="28"/>
+      <c r="DV203" s="28"/>
+      <c r="DW203" s="28"/>
+      <c r="EC203" s="28"/>
+      <c r="ED203" s="28"/>
+      <c r="EJ203" s="28"/>
+      <c r="EK203" s="28"/>
+      <c r="EQ203" s="28"/>
+      <c r="ER203" s="28"/>
+      <c r="EX203" s="28"/>
+      <c r="EY203" s="28"/>
+      <c r="FE203" s="28"/>
+      <c r="FF203" s="28"/>
+      <c r="FL203" s="28"/>
+      <c r="FM203" s="28"/>
+      <c r="FS203" s="28"/>
+      <c r="FT203" s="28"/>
+      <c r="FZ203" s="28"/>
+      <c r="GA203" s="28"/>
+      <c r="GG203" s="28"/>
+      <c r="GH203" s="28"/>
+      <c r="GN203" s="28"/>
+      <c r="GO203" s="28"/>
+      <c r="GU203" s="28"/>
+      <c r="GV203" s="28"/>
+      <c r="HB203" s="28"/>
+      <c r="HC203" s="28"/>
+      <c r="HI203" s="28"/>
+      <c r="HJ203" s="28"/>
+      <c r="HP203" s="28"/>
+      <c r="HQ203" s="28"/>
+      <c r="HW203" s="28"/>
+      <c r="HX203" s="28"/>
+      <c r="ID203" s="28"/>
+      <c r="IE203" s="28"/>
+      <c r="IK203" s="28"/>
+      <c r="IL203" s="28"/>
+      <c r="IR203" s="28"/>
+      <c r="IS203" s="28"/>
+      <c r="IY203" s="28"/>
+      <c r="IZ203" s="28"/>
+      <c r="JF203" s="28"/>
+      <c r="JG203" s="28"/>
+      <c r="JM203" s="28"/>
+      <c r="JN203" s="28"/>
+      <c r="JT203" s="28"/>
+      <c r="JU203" s="28"/>
+      <c r="KA203" s="28"/>
+      <c r="KB203" s="28"/>
+      <c r="KH203" s="28"/>
+      <c r="KI203" s="28"/>
+      <c r="KO203" s="28"/>
+      <c r="KP203" s="28"/>
+      <c r="KV203" s="28"/>
+      <c r="KW203" s="28"/>
+      <c r="LC203" s="28"/>
+      <c r="LD203" s="28"/>
+      <c r="LJ203" s="28"/>
+      <c r="LK203" s="28"/>
+    </row>
+    <row r="204" spans="1:323" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="25"/>
+      <c r="B204" s="26"/>
+      <c r="C204" s="53"/>
+      <c r="D204" s="29"/>
+      <c r="E204" s="13"/>
+      <c r="F204" s="13"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="5"/>
+      <c r="N204" s="28"/>
+      <c r="O204" s="28"/>
+      <c r="U204" s="28"/>
+      <c r="V204" s="28"/>
+      <c r="AB204" s="28"/>
+      <c r="AC204" s="28"/>
+      <c r="AI204" s="28"/>
+      <c r="AJ204" s="28"/>
+      <c r="AP204" s="28"/>
+      <c r="AQ204" s="28"/>
+      <c r="AW204" s="28"/>
+      <c r="AX204" s="28"/>
+      <c r="BD204" s="28"/>
+      <c r="BE204" s="28"/>
+      <c r="BK204" s="28"/>
+      <c r="BL204" s="28"/>
+      <c r="BR204" s="28"/>
+      <c r="BS204" s="28"/>
+      <c r="BY204" s="28"/>
+      <c r="BZ204" s="28"/>
+      <c r="CE204" s="38"/>
+      <c r="CF204" s="28"/>
+      <c r="CG204" s="28"/>
+      <c r="CM204" s="28"/>
+      <c r="CN204" s="28"/>
+      <c r="CT204" s="28"/>
+      <c r="CU204" s="28"/>
+      <c r="DA204" s="28"/>
+      <c r="DB204" s="28"/>
+      <c r="DH204" s="28"/>
+      <c r="DI204" s="28"/>
+      <c r="DO204" s="28"/>
+      <c r="DP204" s="28"/>
+      <c r="DV204" s="28"/>
+      <c r="DW204" s="28"/>
+      <c r="EC204" s="28"/>
+      <c r="ED204" s="28"/>
+      <c r="EJ204" s="28"/>
+      <c r="EK204" s="28"/>
+      <c r="EQ204" s="28"/>
+      <c r="ER204" s="28"/>
+      <c r="EX204" s="28"/>
+      <c r="EY204" s="28"/>
+      <c r="FE204" s="28"/>
+      <c r="FF204" s="28"/>
+      <c r="FL204" s="28"/>
+      <c r="FM204" s="28"/>
+      <c r="FS204" s="28"/>
+      <c r="FT204" s="28"/>
+      <c r="FZ204" s="28"/>
+      <c r="GA204" s="28"/>
+      <c r="GG204" s="28"/>
+      <c r="GH204" s="28"/>
+      <c r="GN204" s="28"/>
+      <c r="GO204" s="28"/>
+      <c r="GU204" s="28"/>
+      <c r="GV204" s="28"/>
+      <c r="HB204" s="28"/>
+      <c r="HC204" s="28"/>
+      <c r="HI204" s="28"/>
+      <c r="HJ204" s="28"/>
+      <c r="HP204" s="28"/>
+      <c r="HQ204" s="28"/>
+      <c r="HW204" s="28"/>
+      <c r="HX204" s="28"/>
+      <c r="ID204" s="28"/>
+      <c r="IE204" s="28"/>
+      <c r="IK204" s="28"/>
+      <c r="IL204" s="28"/>
+      <c r="IR204" s="28"/>
+      <c r="IS204" s="28"/>
+      <c r="IY204" s="28"/>
+      <c r="IZ204" s="28"/>
+      <c r="JF204" s="28"/>
+      <c r="JG204" s="28"/>
+      <c r="JM204" s="28"/>
+      <c r="JN204" s="28"/>
+      <c r="JT204" s="28"/>
+      <c r="JU204" s="28"/>
+      <c r="KA204" s="28"/>
+      <c r="KB204" s="28"/>
+      <c r="KH204" s="28"/>
+      <c r="KI204" s="28"/>
+      <c r="KO204" s="28"/>
+      <c r="KP204" s="28"/>
+      <c r="KV204" s="28"/>
+      <c r="KW204" s="28"/>
+      <c r="LC204" s="28"/>
+      <c r="LD204" s="28"/>
+      <c r="LJ204" s="28"/>
+      <c r="LK204" s="28"/>
+    </row>
+    <row r="205" spans="1:323" x14ac:dyDescent="0.25">
+      <c r="A205" s="14"/>
+      <c r="B205" s="14"/>
+      <c r="CE205" s="38"/>
+      <c r="CG205" s="38"/>
+      <c r="CI205" s="38"/>
+      <c r="CK205" s="38"/>
+    </row>
+    <row r="208" spans="1:323" x14ac:dyDescent="0.25">
+      <c r="C208" s="56"/>
     </row>
   </sheetData>
   <sortState ref="A130:LK164">
     <sortCondition descending="1" ref="B130:B164"/>
   </sortState>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B192:C192"/>
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A2:C4"/>
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A125:C125"/>
     <mergeCell ref="B164:C164"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU190 DJ8:DN190 DC8:DG190 EE8:EI190 CA8:CE190 AY8:BC190 AR8:AV190 AK8:AO190 AD8:AH190 BF66:BJ190 BM66:BQ190 BT66:BX190 W78:AA190 P60:T190 CV60:CZ190 CO69:CS190 DX114:EB190 CH60:CL190 EL8:EP190 ES8:EW190 EZ8:FD190 FG8:FK190 FN8:FR190 FU8:FY190 GB8:GF190 GI8:GM190 GP8:GT190 GW8:HA190 J69:M190 HD129:HH190 HK129:HO190 HR129:HV190 HY129:IC190 IF129:IJ190 IM129:IQ190 IT129:IX190 JA129:JE190 JH129:JL190 JO129:JS190 JV129:JZ190 KC129:KG190 KJ129:KN190 KQ129:KU190 KX129:LB190 LE129:LI190">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU204 DJ8:DN204 DC8:DG204 EE8:EI204 CA8:CE204 AY8:BC204 AR8:AV204 AK8:AO204 AD8:AH204 BF66:BJ204 BM66:BQ204 BT66:BX204 W78:AA204 P60:T204 CV60:CZ204 CO69:CS204 DX114:EB204 CH60:CL204 EL8:EP204 ES8:EW204 EZ8:FD204 FG8:FK204 FN8:FR204 FU8:FY204 GB8:GF204 GI8:GM204 GP8:GT204 GW8:HA204 J69:M204 HD129:HH204 HK129:HO204 HR129:HV204 HY129:IC204 IF129:IJ204 IM129:IQ204 IT129:IX204 JA129:JE204 JH129:JL204 JO129:JS204 JV129:JZ204 KC129:KG204 KJ129:KN204 KQ129:KU204 KX129:LB204 LE129:LI204">
     <cfRule type="expression" dxfId="176" priority="268">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -26657,7 +28095,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A191:HC191">
+  <conditionalFormatting sqref="A205:HC205">
     <cfRule type="expression" dxfId="168" priority="267">
       <formula>TRUE</formula>
     </cfRule>
@@ -26719,7 +28157,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HD191:HJ191">
+  <conditionalFormatting sqref="HD205:HJ205">
     <cfRule type="expression" dxfId="150" priority="160">
       <formula>TRUE</formula>
     </cfRule>
@@ -26750,7 +28188,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HK191:HQ191">
+  <conditionalFormatting sqref="HK205:HQ205">
     <cfRule type="expression" dxfId="141" priority="150">
       <formula>TRUE</formula>
     </cfRule>
@@ -26781,7 +28219,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HR191:HX191">
+  <conditionalFormatting sqref="HR205:HX205">
     <cfRule type="expression" dxfId="132" priority="140">
       <formula>TRUE</formula>
     </cfRule>
@@ -26812,7 +28250,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HY191:IE191">
+  <conditionalFormatting sqref="HY205:IE205">
     <cfRule type="expression" dxfId="123" priority="130">
       <formula>TRUE</formula>
     </cfRule>
@@ -26843,7 +28281,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IF191:IL191">
+  <conditionalFormatting sqref="IF205:IL205">
     <cfRule type="expression" dxfId="114" priority="120">
       <formula>TRUE</formula>
     </cfRule>
@@ -26874,7 +28312,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM191:IS191">
+  <conditionalFormatting sqref="IM205:IS205">
     <cfRule type="expression" dxfId="105" priority="110">
       <formula>TRUE</formula>
     </cfRule>
@@ -26905,7 +28343,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IT191:IZ191">
+  <conditionalFormatting sqref="IT205:IZ205">
     <cfRule type="expression" dxfId="96" priority="100">
       <formula>TRUE</formula>
     </cfRule>
@@ -26936,7 +28374,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="JA191:JG191">
+  <conditionalFormatting sqref="JA205:JG205">
     <cfRule type="expression" dxfId="87" priority="90">
       <formula>TRUE</formula>
     </cfRule>
@@ -26967,7 +28405,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="JH191:JN191">
+  <conditionalFormatting sqref="JH205:JN205">
     <cfRule type="expression" dxfId="78" priority="80">
       <formula>TRUE</formula>
     </cfRule>
@@ -26998,7 +28436,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="JO191:JU191">
+  <conditionalFormatting sqref="JO205:JU205">
     <cfRule type="expression" dxfId="69" priority="70">
       <formula>TRUE</formula>
     </cfRule>
@@ -27029,7 +28467,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="JV191:KB191">
+  <conditionalFormatting sqref="JV205:KB205">
     <cfRule type="expression" dxfId="60" priority="60">
       <formula>TRUE</formula>
     </cfRule>
@@ -27060,7 +28498,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="KC191:KI191">
+  <conditionalFormatting sqref="KC205:KI205">
     <cfRule type="expression" dxfId="51" priority="50">
       <formula>TRUE</formula>
     </cfRule>
@@ -27091,7 +28529,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="KJ191:KP191">
+  <conditionalFormatting sqref="KJ205:KP205">
     <cfRule type="expression" dxfId="42" priority="40">
       <formula>TRUE</formula>
     </cfRule>
@@ -27122,7 +28560,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="KQ191:KW191">
+  <conditionalFormatting sqref="KQ205:KW205">
     <cfRule type="expression" dxfId="33" priority="30">
       <formula>TRUE</formula>
     </cfRule>
@@ -27153,7 +28591,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="KX191:LD191">
+  <conditionalFormatting sqref="KX205:LD205">
     <cfRule type="expression" dxfId="24" priority="20">
       <formula>TRUE</formula>
     </cfRule>
@@ -27184,7 +28622,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="LE191:LK191">
+  <conditionalFormatting sqref="LE205:LK205">
     <cfRule type="expression" dxfId="15" priority="10">
       <formula>TRUE</formula>
     </cfRule>
@@ -27254,9 +28692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AO238"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27331,10 +28769,10 @@
         <v>41690</v>
       </c>
       <c r="C6" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="36" t="s">
         <v>161</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>162</v>
       </c>
       <c r="E6" s="61"/>
       <c r="AO6" s="35" t="s">
@@ -27349,16 +28787,16 @@
         <v>41705</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AO7" s="35" t="s">
         <v>56</v>
@@ -27372,16 +28810,16 @@
         <v>41705</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
@@ -27392,16 +28830,16 @@
         <v>41724</v>
       </c>
       <c r="C9" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>185</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>186</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
@@ -27412,10 +28850,10 @@
         <v>41738</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>56</v>
@@ -27429,16 +28867,16 @@
         <v>41751</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -27449,16 +28887,16 @@
         <v>41795</v>
       </c>
       <c r="C12" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="36" t="s">
         <v>203</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>204</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
@@ -27469,16 +28907,16 @@
         <v>41810</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
@@ -27489,11 +28927,15 @@
         <v>41815</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>237</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="67"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="36">

</xml_diff>